<commit_message>
picrust reinstall ete, 4 book corrected
</commit_message>
<xml_diff>
--- a/data_Ref/bacteria_corrosion_summary_improved.xlsx
+++ b/data_Ref/bacteria_corrosion_summary_improved.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,7 +508,7 @@
       <c r="H2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="b">
+      <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="inlineStr"/>
@@ -534,7 +534,7 @@
       <c r="H3" t="n">
         <v>0</v>
       </c>
-      <c r="I3" t="b">
+      <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="inlineStr"/>
@@ -560,7 +560,7 @@
       <c r="H4" t="n">
         <v>0</v>
       </c>
-      <c r="I4" t="b">
+      <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="inlineStr"/>
@@ -586,7 +586,7 @@
       <c r="H5" t="n">
         <v>0</v>
       </c>
-      <c r="I5" t="b">
+      <c r="I5" t="n">
         <v>0</v>
       </c>
       <c r="J5" t="inlineStr"/>
@@ -612,7 +612,7 @@
       <c r="H6" t="n">
         <v>0</v>
       </c>
-      <c r="I6" t="b">
+      <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -638,7 +638,7 @@
       <c r="H7" t="n">
         <v>0</v>
       </c>
-      <c r="I7" t="b">
+      <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -664,7 +664,7 @@
       <c r="H8" t="n">
         <v>0</v>
       </c>
-      <c r="I8" t="b">
+      <c r="I8" t="n">
         <v>0</v>
       </c>
       <c r="J8" t="inlineStr"/>
@@ -690,7 +690,7 @@
       <c r="H9" t="n">
         <v>0</v>
       </c>
-      <c r="I9" t="b">
+      <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="inlineStr"/>
@@ -716,7 +716,7 @@
       <c r="H10" t="n">
         <v>0</v>
       </c>
-      <c r="I10" t="b">
+      <c r="I10" t="n">
         <v>0</v>
       </c>
       <c r="J10" t="inlineStr"/>
@@ -742,7 +742,7 @@
       <c r="H11" t="n">
         <v>0</v>
       </c>
-      <c r="I11" t="b">
+      <c r="I11" t="n">
         <v>0</v>
       </c>
       <c r="J11" t="inlineStr"/>
@@ -768,7 +768,7 @@
       <c r="H12" t="n">
         <v>0</v>
       </c>
-      <c r="I12" t="b">
+      <c r="I12" t="n">
         <v>0</v>
       </c>
       <c r="J12" t="inlineStr"/>
@@ -794,7 +794,7 @@
       <c r="H13" t="n">
         <v>0</v>
       </c>
-      <c r="I13" t="b">
+      <c r="I13" t="n">
         <v>0</v>
       </c>
       <c r="J13" t="inlineStr"/>
@@ -820,7 +820,7 @@
       <c r="H14" t="n">
         <v>0</v>
       </c>
-      <c r="I14" t="b">
+      <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="inlineStr"/>
@@ -846,7 +846,7 @@
       <c r="H15" t="n">
         <v>0</v>
       </c>
-      <c r="I15" t="b">
+      <c r="I15" t="n">
         <v>0</v>
       </c>
       <c r="J15" t="inlineStr"/>
@@ -872,7 +872,7 @@
       <c r="H16" t="n">
         <v>0</v>
       </c>
-      <c r="I16" t="b">
+      <c r="I16" t="n">
         <v>0</v>
       </c>
       <c r="J16" t="inlineStr"/>
@@ -898,7 +898,7 @@
       <c r="H17" t="n">
         <v>0</v>
       </c>
-      <c r="I17" t="b">
+      <c r="I17" t="n">
         <v>0</v>
       </c>
       <c r="J17" t="inlineStr"/>
@@ -924,7 +924,7 @@
       <c r="H18" t="n">
         <v>0</v>
       </c>
-      <c r="I18" t="b">
+      <c r="I18" t="n">
         <v>0</v>
       </c>
       <c r="J18" t="inlineStr"/>
@@ -950,7 +950,7 @@
       <c r="H19" t="n">
         <v>0</v>
       </c>
-      <c r="I19" t="b">
+      <c r="I19" t="n">
         <v>0</v>
       </c>
       <c r="J19" t="inlineStr"/>
@@ -976,7 +976,7 @@
       <c r="H20" t="n">
         <v>0</v>
       </c>
-      <c r="I20" t="b">
+      <c r="I20" t="n">
         <v>0</v>
       </c>
       <c r="J20" t="inlineStr"/>
@@ -1002,7 +1002,7 @@
       <c r="H21" t="n">
         <v>0</v>
       </c>
-      <c r="I21" t="b">
+      <c r="I21" t="n">
         <v>0</v>
       </c>
       <c r="J21" t="inlineStr"/>
@@ -1028,7 +1028,7 @@
       <c r="H22" t="n">
         <v>0</v>
       </c>
-      <c r="I22" t="b">
+      <c r="I22" t="n">
         <v>0</v>
       </c>
       <c r="J22" t="inlineStr"/>
@@ -1054,7 +1054,7 @@
       <c r="H23" t="n">
         <v>0</v>
       </c>
-      <c r="I23" t="b">
+      <c r="I23" t="n">
         <v>0</v>
       </c>
       <c r="J23" t="inlineStr"/>
@@ -1080,7 +1080,7 @@
       <c r="H24" t="n">
         <v>0</v>
       </c>
-      <c r="I24" t="b">
+      <c r="I24" t="n">
         <v>0</v>
       </c>
       <c r="J24" t="inlineStr"/>
@@ -1106,7 +1106,7 @@
       <c r="H25" t="n">
         <v>0</v>
       </c>
-      <c r="I25" t="b">
+      <c r="I25" t="n">
         <v>0</v>
       </c>
       <c r="J25" t="inlineStr"/>
@@ -1132,7 +1132,7 @@
       <c r="H26" t="n">
         <v>0</v>
       </c>
-      <c r="I26" t="b">
+      <c r="I26" t="n">
         <v>0</v>
       </c>
       <c r="J26" t="inlineStr"/>
@@ -1158,7 +1158,7 @@
       <c r="H27" t="n">
         <v>0</v>
       </c>
-      <c r="I27" t="b">
+      <c r="I27" t="n">
         <v>0</v>
       </c>
       <c r="J27" t="inlineStr"/>
@@ -1184,7 +1184,7 @@
       <c r="H28" t="n">
         <v>0</v>
       </c>
-      <c r="I28" t="b">
+      <c r="I28" t="n">
         <v>0</v>
       </c>
       <c r="J28" t="inlineStr"/>
@@ -1210,7 +1210,7 @@
       <c r="H29" t="n">
         <v>0</v>
       </c>
-      <c r="I29" t="b">
+      <c r="I29" t="n">
         <v>0</v>
       </c>
       <c r="J29" t="inlineStr"/>
@@ -1236,7 +1236,7 @@
       <c r="H30" t="n">
         <v>0</v>
       </c>
-      <c r="I30" t="b">
+      <c r="I30" t="n">
         <v>0</v>
       </c>
       <c r="J30" t="inlineStr"/>
@@ -1262,16 +1262,14 @@
       <c r="H31" t="n">
         <v>0</v>
       </c>
-      <c r="I31" t="b">
+      <c r="I31" t="n">
         <v>0</v>
       </c>
       <c r="J31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>727</t>
-        </is>
+      <c r="A32" s="1" t="n">
+        <v>727</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1290,10 +1288,1106 @@
       <c r="H32" t="n">
         <v>0</v>
       </c>
-      <c r="I32" t="b">
+      <c r="I32" t="n">
         <v>0</v>
       </c>
       <c r="J32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Anaerococcus</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E33" t="n">
+        <v>11</v>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Anaerococcus</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E34" t="n">
+        <v>11</v>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Anaerococcus</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E35" t="n">
+        <v>11</v>
+      </c>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Anaerococcus</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E36" t="n">
+        <v>11</v>
+      </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Aquamicrobium</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Azospira</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="E38" t="n">
+        <v>25</v>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Brachybacterium</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="E39" t="n">
+        <v>6</v>
+      </c>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Brevibacterium</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation; sulfate_reduction; acid_production</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>42.40000000000001</v>
+      </c>
+      <c r="E40" t="n">
+        <v>76</v>
+      </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Bulleidia</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>metal_reduction</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Cellulosimicrobium</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="E42" t="n">
+        <v>9</v>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Clavibacter</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation; sulfate_reduction; acid_production</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>24.7</v>
+      </c>
+      <c r="E43" t="n">
+        <v>38</v>
+      </c>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Clostridium</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>636.1</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1905</v>
+      </c>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Anaerococcus</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E45" t="n">
+        <v>11</v>
+      </c>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Aquamicrobium</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Azospira</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="E47" t="n">
+        <v>25</v>
+      </c>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Brachybacterium</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="E48" t="n">
+        <v>6</v>
+      </c>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Brevibacterium</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation; sulfate_reduction; acid_production</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>42.40000000000001</v>
+      </c>
+      <c r="E49" t="n">
+        <v>76</v>
+      </c>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Bulleidia</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>metal_reduction</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Cellulosimicrobium</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="E51" t="n">
+        <v>9</v>
+      </c>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Clavibacter</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation; sulfate_reduction; acid_production</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>24.7</v>
+      </c>
+      <c r="E52" t="n">
+        <v>38</v>
+      </c>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Clostridium</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>636.1</v>
+      </c>
+      <c r="E53" t="n">
+        <v>1905</v>
+      </c>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Cohnella</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="E54" t="n">
+        <v>4</v>
+      </c>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Corynebacterium</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>215.5</v>
+      </c>
+      <c r="E55" t="n">
+        <v>609</v>
+      </c>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Enterococcus</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation; sulfate_reduction; acid_production</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>1534</v>
+      </c>
+      <c r="E56" t="n">
+        <v>4974</v>
+      </c>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>354</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Halomonas</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation; sulfate_reduction; acid_production</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>64.59999999999999</v>
+      </c>
+      <c r="E57" t="n">
+        <v>91</v>
+      </c>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>408</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Legionella</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>165</v>
+      </c>
+      <c r="E58" t="n">
+        <v>396</v>
+      </c>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>456</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Methyloversatilis</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="E59" t="n">
+        <v>9</v>
+      </c>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>470</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Mycobacterium</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>1411.6</v>
+      </c>
+      <c r="E60" t="n">
+        <v>4577</v>
+      </c>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>471</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Mycoplana</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>474</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Neisseria</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>435.1</v>
+      </c>
+      <c r="E62" t="n">
+        <v>1359</v>
+      </c>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>491</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Novosphingobium</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>15.9</v>
+      </c>
+      <c r="E63" t="n">
+        <v>20</v>
+      </c>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>497</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Oerskovia</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1</v>
+      </c>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>503</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Opitutus</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E65" t="n">
+        <v>4</v>
+      </c>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>512</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Oxobacter</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>526</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Paracoccus</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation; sulfate_reduction; acid_production</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>121.6</v>
+      </c>
+      <c r="E67" t="n">
+        <v>298</v>
+      </c>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>566</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Prevotella</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>acid_production; metal_reduction; biofilm_formation; sulfate_reduction</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>188.5</v>
+      </c>
+      <c r="E68" t="n">
+        <v>530</v>
+      </c>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>581</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Psb-m-3</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>metal_reduction</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" t="n">
+        <v>1</v>
+      </c>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>583</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Pseudarthrobacter</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="E70" t="n">
+        <v>4</v>
+      </c>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>584</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Pseudoalteromonas</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>69.39999999999999</v>
+      </c>
+      <c r="E71" t="n">
+        <v>129</v>
+      </c>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>621</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Roseateles</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="E72" t="n">
+        <v>5</v>
+      </c>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr"/>
+      <c r="J72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>687</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Streptococcus</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation; sulfate_reduction; acid_production</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>3014.8</v>
+      </c>
+      <c r="E73" t="n">
+        <v>9850</v>
+      </c>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>727</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Thiobacillus</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>metal_reduction; acid_production; sulfate_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>180.1</v>
+      </c>
+      <c r="E74" t="n">
+        <v>430</v>
+      </c>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>30414.1</v>
+      </c>
+      <c r="E75" t="n">
+        <v>100896</v>
+      </c>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1306,7 +2400,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1885,10 +2979,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>727</t>
-        </is>
+      <c r="A32" s="1" t="n">
+        <v>727</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1903,6 +2995,836 @@
       <c r="D32" s="2" t="inlineStr">
         <is>
           <t>The aim of this study was to develop new sulfur-copolymer concrete composites using waste compounds that have good mechanical characteristics and show a resistance to biocorrosion. The comonomers used to synthesize the sulfur-organic copolymers were-90 wt. % sulfur; 5 wt. % dicyclopentadiene (DCPD); 5 wt. % organic monomers, styrene (SDS), 1-decene (SDD), turpentine (SDT), and furfural (SDF). The concrete composites based on sulfur-organic copolymers were filled with aggregates, sand, gravel, as well as additives and industrial waste such as fly ash or phosphogypsum. The sulfur-organic copolymers were found to be chemically stable (softening temperature, thermal stability, melting temperature, amount of recrystallized sulfur, and shore D hardness). Partial replacement of DCPD with other organic comonomers did not change the thermal stability markedly but did make the copolymers more elastic. However, the materials became significantly stiffer after repeated melting. All the tested copolymers were found to be resistant to microbial corrosion. The highest resistance was exhibited by the SDS-containing polymer, while the SDF polymer exhibited the greatest change due to the activity of the microorganisms (FTIR analysis and sulfur crystallization). The concrete composites with sulfur-organic copolymers containing DCPD, SDS, SDF, fly ash, and phosphogypsum were mechanically resistant to compression and stretching, had low water absorbance, and were resistant to factors, such as temperature and salt. Resistance to freezing and thawing (150 cycles) was not confirmed. The concrete composites with sulfur-organic copolymers showed resistance to bacterial growth and acid activity during 8 weeks of incubation with microorganisms. No significant structural changes were observed in the SDS composites after incubation with bacteria, whereas composites containing SDF showed slight changes (FTIR and microscopic analysis). The concrete composite containing sulfur, DCPD, SDS, sand, gravel, and fly ash was the most resistant to microbiological corrosion, based on the metabolic activity of the bacteria and the production of ergosterol by the molds after eight weeks of incubation. It was found that &lt;i&gt;Thiobacillus thioparus&lt;/i&gt; was the first of the acidifying bacteria to colonize the sulfur concrete, decreasing the pH of the environment. The molds &lt;i&gt;Penicillium chrysogenum&lt;/i&gt;, &lt;i&gt;Aspergillus versicolor&lt;/i&gt; and &lt;i&gt;Cladosporium herbarum&lt;/i&gt; were able to grow on the surface of the tested composites only in the presence of an organic carbon source (glucose). During incubation, they produced organic acids and acidified the environment. However, no morphological changes in the concretes were observed suggesting that sulfur-organic copolymers containing styrene could be used as engineering materials or be applied as binders in sulfur-concretes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Anaerococcus</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="inlineStr">
+        <is>
+          <t>Akgül, Ö., Söyletir, G. &amp; Ülger Toprak, N. (2020). [Antimicrobial Susceptibility of Pathogenic Gram-positive Anaerobic Cocci: Data of a University Hospital in Turkey].. Mikrobiyoloji bulteni, 54(3), 404-417.</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>Gram-positive anaerobic cocci (GPAC), a large group of anaerobic bacteria, are the members of the normal microbiota that colonizes the skin and mucosal surfaces of the human body. However, in case of a wound or when the host becomes immunocompromised, GPAC can cause invasive and most frequently mixed infections. GPAC are the second most frequently isolated bacteria in anaerobic infections. Although the studies are limited, GPAC have been reported to develop resistance to antimicrobial drugs. The resistance of the pathogens to the antimicrobials and improper therapy can cause poor clinical outcomes. Therefore, monitoring of the resistance trends of regional clinically important anaerobic bacteria periodically is recommended. In our study, we aimed to determine the antimicrobial susceptibility profiles of clinically important GPAC. A total of 100 non-duplicated pathogenic GPAC isolates were collected from Marmara University Hospital between 2013 and 2015. The isolates were identified by using conventional methods, "matrix-assisted laser desorption ionization-time of flight mass spectrometry system (MALDI-TOF MS)" (VITEK MS; v3.0, bioMerieux, France) and 16S rRNA gene sequencing. Antimicrobial susceptibility test was carried out by the agar dilution method according to the Clinical and Laboratory Standards Institute (CLSI) guidelines. The following antimicrobials were tested: penicillin, amoxicillin/ clavulanic acid (AMC), cefoxitin, meropenem, clindamycin, erythromycin, tetracycline, tigecycline, chloramphenicol, moxifloxacin and metronidazole. The minimum inhibitory concentration (MIC) results were interpreted according to the breakpoints described by the European Committee on Antimicrobial Susceptibility Testing (EUCAST). Breakpoints recommended by CLSI for cefoxitin, tetracycline and moxifloxacin, and breakpoint recommended by Food and Drug Administration (FDA) for tigecycline were used since there were no EUCAST breakpoints for these antimicrobials. MIC50 and MIC90 values were determined for erythromycin since the breakpoint was not described by EUCAST, CLSI or FDA guidelines. The identification results showed that the strains (n= 100) consisted of five different GPAC genus; Parvomonas (40%), Finegoldia (34%), Peptoniphilus (14%), Peptostreptococcus (10%) and Anaerococcus (1%). All of the organisms were susceptible to meropenem, tigecycline and metronidazole. The isolates were highly susceptible to penicillin, AMC, cefoxitin, and chloramphenicol, since the resistance rates against these antimicrobials were 5% or less. The resistance rates against clindamycin, tetracycline and moxifloxacin were 14%, 31% and 24%, respectively. In total, 11% of the isolates were multidrug resistant. Metronidazole and tigecycline displayed high in vitro activity against GPAC and both are appropriate antimicrobials for the selection of empiric therapy. The effectiveness of meropenem was also found high, but it was observed that this antimicrobial would be more appropriate to use in the treatment of severe mixed infections accompanied by other microorganisms with the resistance potential. Detection of penicillin and AMC resistant isolates, which are frequently used in the treatment of GPAC infection, requires periodic monitoring of the antimicrobial susceptibility patterns of GPAC. The high rates of resistance against clindamycin, tetracycline and moksifloxacin indicated that these antimicrobials should not be used for empirical treatment of infections without prior antimicrobial susceptibility testing. This study is one of the largest susceptibility studies specifically carried out on GPAC to date in Turkey. We believe that our results will provide good surveillance data both for our hospital and our country.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Anaerococcus</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
+          <t>Akgül, Ö., Söyletir, G. &amp; Ülger Toprak, N. (2020). [Antimicrobial Susceptibility of Pathogenic Gram-positive Anaerobic Cocci: Data of a University Hospital in Turkey].. Mikrobiyoloji bulteni, 54(3), 404-417.</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>Gram-positive anaerobic cocci (GPAC), a large group of anaerobic bacteria, are the members of the normal microbiota that colonizes the skin and mucosal surfaces of the human body. However, in case of a wound or when the host becomes immunocompromised, GPAC can cause invasive and most frequently mixed infections. GPAC are the second most frequently isolated bacteria in anaerobic infections. Although the studies are limited, GPAC have been reported to develop resistance to antimicrobial drugs. The resistance of the pathogens to the antimicrobials and improper therapy can cause poor clinical outcomes. Therefore, monitoring of the resistance trends of regional clinically important anaerobic bacteria periodically is recommended. In our study, we aimed to determine the antimicrobial susceptibility profiles of clinically important GPAC. A total of 100 non-duplicated pathogenic GPAC isolates were collected from Marmara University Hospital between 2013 and 2015. The isolates were identified by using conventional methods, "matrix-assisted laser desorption ionization-time of flight mass spectrometry system (MALDI-TOF MS)" (VITEK MS; v3.0, bioMerieux, France) and 16S rRNA gene sequencing. Antimicrobial susceptibility test was carried out by the agar dilution method according to the Clinical and Laboratory Standards Institute (CLSI) guidelines. The following antimicrobials were tested: penicillin, amoxicillin/ clavulanic acid (AMC), cefoxitin, meropenem, clindamycin, erythromycin, tetracycline, tigecycline, chloramphenicol, moxifloxacin and metronidazole. The minimum inhibitory concentration (MIC) results were interpreted according to the breakpoints described by the European Committee on Antimicrobial Susceptibility Testing (EUCAST). Breakpoints recommended by CLSI for cefoxitin, tetracycline and moxifloxacin, and breakpoint recommended by Food and Drug Administration (FDA) for tigecycline were used since there were no EUCAST breakpoints for these antimicrobials. MIC50 and MIC90 values were determined for erythromycin since the breakpoint was not described by EUCAST, CLSI or FDA guidelines. The identification results showed that the strains (n= 100) consisted of five different GPAC genus; Parvomonas (40%), Finegoldia (34%), Peptoniphilus (14%), Peptostreptococcus (10%) and Anaerococcus (1%). All of the organisms were susceptible to meropenem, tigecycline and metronidazole. The isolates were highly susceptible to penicillin, AMC, cefoxitin, and chloramphenicol, since the resistance rates against these antimicrobials were 5% or less. The resistance rates against clindamycin, tetracycline and moxifloxacin were 14%, 31% and 24%, respectively. In total, 11% of the isolates were multidrug resistant. Metronidazole and tigecycline displayed high in vitro activity against GPAC and both are appropriate antimicrobials for the selection of empiric therapy. The effectiveness of meropenem was also found high, but it was observed that this antimicrobial would be more appropriate to use in the treatment of severe mixed infections accompanied by other microorganisms with the resistance potential. Detection of penicillin and AMC resistant isolates, which are frequently used in the treatment of GPAC infection, requires periodic monitoring of the antimicrobial susceptibility patterns of GPAC. The high rates of resistance against clindamycin, tetracycline and moksifloxacin indicated that these antimicrobials should not be used for empirical treatment of infections without prior antimicrobial susceptibility testing. This study is one of the largest susceptibility studies specifically carried out on GPAC to date in Turkey. We believe that our results will provide good surveillance data both for our hospital and our country.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Anaerococcus</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="inlineStr">
+        <is>
+          <t>Akgül, Ö., Söyletir, G. &amp; Ülger Toprak, N. (2020). [Antimicrobial Susceptibility of Pathogenic Gram-positive Anaerobic Cocci: Data of a University Hospital in Turkey].. Mikrobiyoloji bulteni, 54(3), 404-417.</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>Gram-positive anaerobic cocci (GPAC), a large group of anaerobic bacteria, are the members of the normal microbiota that colonizes the skin and mucosal surfaces of the human body. However, in case of a wound or when the host becomes immunocompromised, GPAC can cause invasive and most frequently mixed infections. GPAC are the second most frequently isolated bacteria in anaerobic infections. Although the studies are limited, GPAC have been reported to develop resistance to antimicrobial drugs. The resistance of the pathogens to the antimicrobials and improper therapy can cause poor clinical outcomes. Therefore, monitoring of the resistance trends of regional clinically important anaerobic bacteria periodically is recommended. In our study, we aimed to determine the antimicrobial susceptibility profiles of clinically important GPAC. A total of 100 non-duplicated pathogenic GPAC isolates were collected from Marmara University Hospital between 2013 and 2015. The isolates were identified by using conventional methods, "matrix-assisted laser desorption ionization-time of flight mass spectrometry system (MALDI-TOF MS)" (VITEK MS; v3.0, bioMerieux, France) and 16S rRNA gene sequencing. Antimicrobial susceptibility test was carried out by the agar dilution method according to the Clinical and Laboratory Standards Institute (CLSI) guidelines. The following antimicrobials were tested: penicillin, amoxicillin/ clavulanic acid (AMC), cefoxitin, meropenem, clindamycin, erythromycin, tetracycline, tigecycline, chloramphenicol, moxifloxacin and metronidazole. The minimum inhibitory concentration (MIC) results were interpreted according to the breakpoints described by the European Committee on Antimicrobial Susceptibility Testing (EUCAST). Breakpoints recommended by CLSI for cefoxitin, tetracycline and moxifloxacin, and breakpoint recommended by Food and Drug Administration (FDA) for tigecycline were used since there were no EUCAST breakpoints for these antimicrobials. MIC50 and MIC90 values were determined for erythromycin since the breakpoint was not described by EUCAST, CLSI or FDA guidelines. The identification results showed that the strains (n= 100) consisted of five different GPAC genus; Parvomonas (40%), Finegoldia (34%), Peptoniphilus (14%), Peptostreptococcus (10%) and Anaerococcus (1%). All of the organisms were susceptible to meropenem, tigecycline and metronidazole. The isolates were highly susceptible to penicillin, AMC, cefoxitin, and chloramphenicol, since the resistance rates against these antimicrobials were 5% or less. The resistance rates against clindamycin, tetracycline and moxifloxacin were 14%, 31% and 24%, respectively. In total, 11% of the isolates were multidrug resistant. Metronidazole and tigecycline displayed high in vitro activity against GPAC and both are appropriate antimicrobials for the selection of empiric therapy. The effectiveness of meropenem was also found high, but it was observed that this antimicrobial would be more appropriate to use in the treatment of severe mixed infections accompanied by other microorganisms with the resistance potential. Detection of penicillin and AMC resistant isolates, which are frequently used in the treatment of GPAC infection, requires periodic monitoring of the antimicrobial susceptibility patterns of GPAC. The high rates of resistance against clindamycin, tetracycline and moksifloxacin indicated that these antimicrobials should not be used for empirical treatment of infections without prior antimicrobial susceptibility testing. This study is one of the largest susceptibility studies specifically carried out on GPAC to date in Turkey. We believe that our results will provide good surveillance data both for our hospital and our country.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Anaerococcus</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>Akgül, Ö., Söyletir, G. &amp; Ülger Toprak, N. (2020). [Antimicrobial Susceptibility of Pathogenic Gram-positive Anaerobic Cocci: Data of a University Hospital in Turkey].. Mikrobiyoloji bulteni, 54(3), 404-417.</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>Gram-positive anaerobic cocci (GPAC), a large group of anaerobic bacteria, are the members of the normal microbiota that colonizes the skin and mucosal surfaces of the human body. However, in case of a wound or when the host becomes immunocompromised, GPAC can cause invasive and most frequently mixed infections. GPAC are the second most frequently isolated bacteria in anaerobic infections. Although the studies are limited, GPAC have been reported to develop resistance to antimicrobial drugs. The resistance of the pathogens to the antimicrobials and improper therapy can cause poor clinical outcomes. Therefore, monitoring of the resistance trends of regional clinically important anaerobic bacteria periodically is recommended. In our study, we aimed to determine the antimicrobial susceptibility profiles of clinically important GPAC. A total of 100 non-duplicated pathogenic GPAC isolates were collected from Marmara University Hospital between 2013 and 2015. The isolates were identified by using conventional methods, "matrix-assisted laser desorption ionization-time of flight mass spectrometry system (MALDI-TOF MS)" (VITEK MS; v3.0, bioMerieux, France) and 16S rRNA gene sequencing. Antimicrobial susceptibility test was carried out by the agar dilution method according to the Clinical and Laboratory Standards Institute (CLSI) guidelines. The following antimicrobials were tested: penicillin, amoxicillin/ clavulanic acid (AMC), cefoxitin, meropenem, clindamycin, erythromycin, tetracycline, tigecycline, chloramphenicol, moxifloxacin and metronidazole. The minimum inhibitory concentration (MIC) results were interpreted according to the breakpoints described by the European Committee on Antimicrobial Susceptibility Testing (EUCAST). Breakpoints recommended by CLSI for cefoxitin, tetracycline and moxifloxacin, and breakpoint recommended by Food and Drug Administration (FDA) for tigecycline were used since there were no EUCAST breakpoints for these antimicrobials. MIC50 and MIC90 values were determined for erythromycin since the breakpoint was not described by EUCAST, CLSI or FDA guidelines. The identification results showed that the strains (n= 100) consisted of five different GPAC genus; Parvomonas (40%), Finegoldia (34%), Peptoniphilus (14%), Peptostreptococcus (10%) and Anaerococcus (1%). All of the organisms were susceptible to meropenem, tigecycline and metronidazole. The isolates were highly susceptible to penicillin, AMC, cefoxitin, and chloramphenicol, since the resistance rates against these antimicrobials were 5% or less. The resistance rates against clindamycin, tetracycline and moxifloxacin were 14%, 31% and 24%, respectively. In total, 11% of the isolates were multidrug resistant. Metronidazole and tigecycline displayed high in vitro activity against GPAC and both are appropriate antimicrobials for the selection of empiric therapy. The effectiveness of meropenem was also found high, but it was observed that this antimicrobial would be more appropriate to use in the treatment of severe mixed infections accompanied by other microorganisms with the resistance potential. Detection of penicillin and AMC resistant isolates, which are frequently used in the treatment of GPAC infection, requires periodic monitoring of the antimicrobial susceptibility patterns of GPAC. The high rates of resistance against clindamycin, tetracycline and moksifloxacin indicated that these antimicrobials should not be used for empirical treatment of infections without prior antimicrobial susceptibility testing. This study is one of the largest susceptibility studies specifically carried out on GPAC to date in Turkey. We believe that our results will provide good surveillance data both for our hospital and our country.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Aquamicrobium</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="inlineStr"/>
+      <c r="D37" s="2" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Azospira</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="inlineStr">
+        <is>
+          <t>Gregoire, P., et al. (2014). Control of sulfidogenesis through bio-oxidation of H2S coupled to (per)chlorate reduction.. Environmental microbiology reports, 6(6), 558-64.</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>We investigated H2S attenuation by dissimilatory perchlorate-reducing bacteria (DPRB). All DPRB tested oxidized H2S coupled to (per)chlorate reduction without sustaining growth. H2S was preferentially utilized over organic electron donors resulting in an enriched (34S)-elemental sulfur product. Electron microscopy revealed elemental sulfur production in the cytoplasm and on the cell surface of the DPRB Azospira suillum. Based on our results, we propose a novel hybrid enzymatic-abiotic mechanism for H2S oxidation similar to that recently proposed for nitrate-dependent Fe(II) oxidation. The results of this study have implications for the control of biosouring and biocorrosion in a range of industrial environments.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Brachybacterium</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="inlineStr">
+        <is>
+          <t>Liu, Y., et al. (2018). Evaluation of compost, vegetable and food waste as amendments to improve the composting of NaOH/NaClO-contaminated poultry manure.. PloS one, 13(10), e0205112.</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>Regular usage of NaOH/NaClO disinfectants results in high sodium salt and alkalinity of poultry manure. This study compared three amendments: vegetable waste (V), food waste (F) and mature compost (C) for their ability to improve the composting of NaOH/NaClO-contaminated poultry manure. C compost resulted in the highest compost temperatures (p&lt;0.001) and greatest reduction in OM, TC, TN and NH4-N (p&lt;0.05). C and V composts were more efficient at lowering extractable-Na (ext-Na) and electrical conductivity (EC) than F (p&lt;0.05). Maturity was primarily indicated by NH4-N, EC and ext-Na. Bacterial dynamics was profoundly influenced by NH4-N, EC and TC, with the decrease leading to discriminate genera shift from Sinibacillus and Thiopseudomonas to Brevbacterium, Brachybacterium, and Microbacterium. These findings suggest that mature compost was more desirable amendment than vegetable and food waste in the composting of NaOH/NaClO-contaminated poultry manure, and the decrease of ext-Na indicated compost maturity but did not influence bacterial dynamics.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Brevibacterium</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="inlineStr">
+        <is>
+          <t>Liu, B., Li, Z., Yang, X., Du, C. &amp; Li, X. (2020). Microbiologically influenced corrosion of X80 pipeline steel by nitrate reducing bacteria in artificial Beijing soil.. Bioelectrochemistry (Amsterdam, Netherlands), 135, 107551.</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>In this work, we investigated microbiologically influenced corrosion (MIC) of X80 pipeline steel caused by nitrate-reducing bacteria Brevibacterium frigoritolerans (B. frigoritolerans) in an artificial Beijing soil using electrochemical measurements and surface analyses under aerobic conditions. The B. frigoritolerans was isolated from the surrounding soil of the X80 pipeline steel specimen in Beijing using culturing and molecular biology techniques. Confocal laser scanning microscopy images showed that the largest pit depth after 14 days due to B. frigoritolerans was approximately 7.16 μm. Electrochemical tests showed that the B. frigoritolerans could change the stability of the corrosion products on the 7th day. Inhomogeneous biofilm and the conductivity of Fe&lt;sub&gt;2&lt;/sub&gt;O&lt;sub&gt;3&lt;/sub&gt; accelerated the corrosion process. The presence of NH&lt;sub&gt;4&lt;/sub&gt;&lt;sup&gt;+&lt;/sup&gt; on the surface of the X80 pipeline steel revealed that the B. frigoritolerans acted as a biological cathode to promote the cathodic reaction.</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Bulleidia</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="inlineStr">
+        <is>
+          <t>Jia, Y., et al. (2021). Association Between Oral Microbiota and Cigarette Smoking in the Chinese Population.. Frontiers in cellular and infection microbiology, 11, 658203.</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>The oral microbiota has been observed to be influenced by cigarette smoking and linked to several human diseases. However, research on the effect of cigarette smoking on the oral microbiota has not been systematically conducted in the Chinese population. We profiled the oral microbiota of 316 healthy subjects in the Chinese population by 16S rRNA gene sequencing. The alpha diversity of oral microbiota was different between never smokers and smokers (&lt;i&gt;P&lt;/i&gt; = 0.002). Several bacterial taxa were first reported to be associated with cigarette smoking by LEfSe analysis, including &lt;i&gt;Moryella&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 1.56E-04), &lt;i&gt;Bulleidia&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 1.65E-06), and &lt;i&gt;Moraxella&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 3.52E-02) at the genus level and &lt;i&gt;Rothia dentocariosa&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 1.55E-02), &lt;i&gt;Prevotella melaninogenica&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 8.48E-08), &lt;i&gt;Prevotella pallens&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 4.13E-03), &lt;i&gt;Bulleidia moorei&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 1.79E-06), &lt;i&gt;Rothia aeria&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 3.83E-06), &lt;i&gt;Actinobacillus parahaemolyticus&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 2.28E-04), and &lt;i&gt;Haemophilus parainfluenzae&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 4.82E-02) at the species level. Two nitrite-producing bacteria that can increase the acidity of the oral cavity, &lt;i&gt;Actinomyces&lt;/i&gt; and &lt;i&gt;Veillonella&lt;/i&gt;, were also enriched in smokers with FDR-adjusted &lt;i&gt;q&lt;/i&gt;-values of 3.62E-06 and 1.10E-06, respectively. Notably, we observed that two acid production-related pathways, amino acid-related enzymes (&lt;i&gt;q&lt;/i&gt; = 6.19E-05) and amino sugar and nucleotide sugar metabolism (&lt;i&gt;q&lt;/i&gt; = 2.63E-06), were increased in smokers by PICRUSt analysis. Finally, the co-occurrence analysis demonstrated that smoker-enriched bacteria were significantly positively associated with each other and were negatively correlated with the bacteria decreased in smokers. Our results suggested that cigarette smoking may affect oral health by creating a different environment by altering bacterial abundance, connections among oral microbiota, and the microbiota and their metabolic function.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Cellulosimicrobium</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="inlineStr">
+        <is>
+          <t>Wyszkowska, J., Borowik, A., Zaborowska, M. &amp; Kucharski, J. (2022). Sensitivity of &lt;i&gt;Zea mays&lt;/i&gt; and Soil Microorganisms to the Toxic Effect of Chromium (VI).. International journal of molecular sciences, 24(1).</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>Chromium is used in many settings, and hence, it can easily enter the natural environment. It exists in several oxidation states. In soil, depending on its oxidation-reduction potential, it can occur in bivalent, trivalent or hexavalent forms. Hexavalent chromium compounds are cancerogenic to humans. The aim of this study was to determine the effect of Cr(VI) on the structure of bacteria and fungi in soil, to find out how this effect is modified by humic acids and to determine the response of &lt;i&gt;Zea mays&lt;/i&gt; to this form of chromium. A pot experiment was conducted to answer the above questions. &lt;i&gt;Zea mays&lt;/i&gt; was sown in natural soil and soil polluted with Cr(VI) in an amount of 60 mg kg&lt;sup&gt;-1&lt;/sup&gt; d.m. Both soils were treated with humic acids in the form of HumiAgra preparation. The ecophysiological and genetic diversity of bacteria and fungi was assayed in soil under maize (not sown with &lt;i&gt;Zea mays&lt;/i&gt;). In addition, the following were determined: yield of maize, greenness index, index of tolerance to chromium, translocation index and accumulation of chromium in the plant. It has been determined that Cr(VI) significantly distorts the growth and development of &lt;i&gt;Zea mays&lt;/i&gt;, while humic acids completely neutralize its toxic effect on the plant. This element had an adverse effect on the development of bacteria of the genera &lt;i&gt;Cellulosimicrobium&lt;/i&gt;, &lt;i&gt;Kaistobacter&lt;/i&gt;, &lt;i&gt;Rhodanobacter&lt;/i&gt;, &lt;i&gt;Rhodoplanes&lt;/i&gt; and &lt;i&gt;Nocardioides&lt;/i&gt; and fungi of the genera &lt;i&gt;Chaetomium and Humicola&lt;/i&gt;. Soil contamination with Cr(VI) significantly diminished the genetic diversity and richness of bacteria and the ecophysiological diversity of fungi. The negative impact of Cr(VI) on the diversity of bacteria and fungi was mollified by &lt;i&gt;Zea mays&lt;/i&gt; and the application of humic acids.</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Clavibacter</t>
+        </is>
+      </c>
+      <c r="C43" s="2" t="inlineStr">
+        <is>
+          <t>Kaplan, M., et al. (2022). Investigation of Antibacterial Properties of Corrosion-Resistant 316L Steel Alloyed with 0.2 wt.% and 0.5 wt.% Ag.. Materials (Basel, Switzerland), 16(1).</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>The article is devoted to the study of melted ingots, plates rolled from them, and the resulting spherical powder made of corrosion-resistant 316L steel with the addition of 0.2 wt.% and 0.5 wt.% Ag. The study of antibacterial properties, microstructure, and distribution of silver concentrations, as well as qualitative analysis of silver content was carried out. The optimal mode of homogenization annealing of the ingot was 1050 °C for 9 h, which leads to the formation of an austenitic structure. It is shown that the addition of a small amount of silver does not affect the formation of the austenitic structure and silver is distributed evenly throughout the volume of the ingot. The austenitic structure also prevails in the plates after rolling. Silver is distributed evenly throughout the entire volume of the plate. It is noted that the addition of 0.2 wt.% Ag does not affect the strength, elongation, and microhardness of steel, and the addition of 0.5 wt.% Ag does not significantly reduce the strength of steel, however, all samples meet the mechanical characteristics according to the ASTM A240 standard. The qualitative chemical composition of samples made of corrosion-resistant steels was confirmed by X-ray fluorescence analysis methods. By the method of energy-dispersion analysis, the presence of a uniform distribution of silver over the entire volume of the powder particle was determined. The particles have a spherical shape with a minimum number of defects. The study of the antibacterial activity of plates and powder shows the presence of a clear antibacterial effect (bacteria of the genus Xanthomonas campestris, Erwinia carotovora, Pseudomonas marginalis, Clavibacter michiganensis) in samples No. 2 and No. 3 with the addition of 0.2 wt.% and 0.5 wt.% Ag.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Clostridium</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="inlineStr">
+        <is>
+          <t>Ramos Monroy, O., Ruiz Ordaz, N., Hernández Gayosso, M., Juárez Ramírez, C. &amp; Galíndez Mayer, J. (2019). The corrosion process caused by the activity of the anaerobic sporulated bacterium Clostridium celerecrescens on API XL 52 steel.. Environmental science and pollution research international, 26(29), 29991-30002.</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>The microbial corrosion of oil and gas pipes is one of the problems occurring in the oil industry. Various mechanisms explaining microbial corrosion have been demonstrated. Commonly, biocorrosion is attributed to sulfate-reducing bacteria. Also, it has recently been reported that microbial species can connect their electron transport system to metal electrodes. In this research, two spore-forming bacteria isolated in different years from a gas pipeline were identified by biochemical techniques and by 16S rDNA amplification, sequencing, and comparison with the NCBI database. Isolates were also compared between them using molecular techniques as the restriction patterns, unique for 16S rDNA (ARDRA), and the profile of the amplified bit from the genomic DNA, using an unspecific primer (RAPD). The results obtained showed that both isolates corresponded to Clostridium celerecrescens with a 99% similarity according to the sequence reported on the NCBI database. Also, the ARDRA and RAPD electrophoretic profiles of both strains were identical, and no plasmids were found in the strains. Thus, it can be settled that this bacterium is persistent in the environment prevailing in gas pipelines. Also, it was demonstrated that the bacterial secretion of organic acids contributes to the pitting and general biocorrosion of API XL 52 steel. The rates of corrosion obtained, approximately after 40 days, were correlated with the presence and metabolic activity of C. celerecrescens on the metallic surfaces.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Anaerococcus</t>
+        </is>
+      </c>
+      <c r="C45" s="2" t="inlineStr">
+        <is>
+          <t>Akgül, Ö., Söyletir, G. &amp; Ülger Toprak, N. (2020). [Antimicrobial Susceptibility of Pathogenic Gram-positive Anaerobic Cocci: Data of a University Hospital in Turkey].. Mikrobiyoloji bulteni, 54(3), 404-417.</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>Gram-positive anaerobic cocci (GPAC), a large group of anaerobic bacteria, are the members of the normal microbiota that colonizes the skin and mucosal surfaces of the human body. However, in case of a wound or when the host becomes immunocompromised, GPAC can cause invasive and most frequently mixed infections. GPAC are the second most frequently isolated bacteria in anaerobic infections. Although the studies are limited, GPAC have been reported to develop resistance to antimicrobial drugs. The resistance of the pathogens to the antimicrobials and improper therapy can cause poor clinical outcomes. Therefore, monitoring of the resistance trends of regional clinically important anaerobic bacteria periodically is recommended. In our study, we aimed to determine the antimicrobial susceptibility profiles of clinically important GPAC. A total of 100 non-duplicated pathogenic GPAC isolates were collected from Marmara University Hospital between 2013 and 2015. The isolates were identified by using conventional methods, "matrix-assisted laser desorption ionization-time of flight mass spectrometry system (MALDI-TOF MS)" (VITEK MS; v3.0, bioMerieux, France) and 16S rRNA gene sequencing. Antimicrobial susceptibility test was carried out by the agar dilution method according to the Clinical and Laboratory Standards Institute (CLSI) guidelines. The following antimicrobials were tested: penicillin, amoxicillin/ clavulanic acid (AMC), cefoxitin, meropenem, clindamycin, erythromycin, tetracycline, tigecycline, chloramphenicol, moxifloxacin and metronidazole. The minimum inhibitory concentration (MIC) results were interpreted according to the breakpoints described by the European Committee on Antimicrobial Susceptibility Testing (EUCAST). Breakpoints recommended by CLSI for cefoxitin, tetracycline and moxifloxacin, and breakpoint recommended by Food and Drug Administration (FDA) for tigecycline were used since there were no EUCAST breakpoints for these antimicrobials. MIC50 and MIC90 values were determined for erythromycin since the breakpoint was not described by EUCAST, CLSI or FDA guidelines. The identification results showed that the strains (n= 100) consisted of five different GPAC genus; Parvomonas (40%), Finegoldia (34%), Peptoniphilus (14%), Peptostreptococcus (10%) and Anaerococcus (1%). All of the organisms were susceptible to meropenem, tigecycline and metronidazole. The isolates were highly susceptible to penicillin, AMC, cefoxitin, and chloramphenicol, since the resistance rates against these antimicrobials were 5% or less. The resistance rates against clindamycin, tetracycline and moxifloxacin were 14%, 31% and 24%, respectively. In total, 11% of the isolates were multidrug resistant. Metronidazole and tigecycline displayed high in vitro activity against GPAC and both are appropriate antimicrobials for the selection of empiric therapy. The effectiveness of meropenem was also found high, but it was observed that this antimicrobial would be more appropriate to use in the treatment of severe mixed infections accompanied by other microorganisms with the resistance potential. Detection of penicillin and AMC resistant isolates, which are frequently used in the treatment of GPAC infection, requires periodic monitoring of the antimicrobial susceptibility patterns of GPAC. The high rates of resistance against clindamycin, tetracycline and moksifloxacin indicated that these antimicrobials should not be used for empirical treatment of infections without prior antimicrobial susceptibility testing. This study is one of the largest susceptibility studies specifically carried out on GPAC to date in Turkey. We believe that our results will provide good surveillance data both for our hospital and our country.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Aquamicrobium</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="inlineStr"/>
+      <c r="D46" s="2" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Azospira</t>
+        </is>
+      </c>
+      <c r="C47" s="2" t="inlineStr">
+        <is>
+          <t>Gregoire, P., et al. (2014). Control of sulfidogenesis through bio-oxidation of H2S coupled to (per)chlorate reduction.. Environmental microbiology reports, 6(6), 558-64.</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>We investigated H2S attenuation by dissimilatory perchlorate-reducing bacteria (DPRB). All DPRB tested oxidized H2S coupled to (per)chlorate reduction without sustaining growth. H2S was preferentially utilized over organic electron donors resulting in an enriched (34S)-elemental sulfur product. Electron microscopy revealed elemental sulfur production in the cytoplasm and on the cell surface of the DPRB Azospira suillum. Based on our results, we propose a novel hybrid enzymatic-abiotic mechanism for H2S oxidation similar to that recently proposed for nitrate-dependent Fe(II) oxidation. The results of this study have implications for the control of biosouring and biocorrosion in a range of industrial environments.</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Brachybacterium</t>
+        </is>
+      </c>
+      <c r="C48" s="2" t="inlineStr">
+        <is>
+          <t>Liu, Y., et al. (2018). Evaluation of compost, vegetable and food waste as amendments to improve the composting of NaOH/NaClO-contaminated poultry manure.. PloS one, 13(10), e0205112.</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>Regular usage of NaOH/NaClO disinfectants results in high sodium salt and alkalinity of poultry manure. This study compared three amendments: vegetable waste (V), food waste (F) and mature compost (C) for their ability to improve the composting of NaOH/NaClO-contaminated poultry manure. C compost resulted in the highest compost temperatures (p&lt;0.001) and greatest reduction in OM, TC, TN and NH4-N (p&lt;0.05). C and V composts were more efficient at lowering extractable-Na (ext-Na) and electrical conductivity (EC) than F (p&lt;0.05). Maturity was primarily indicated by NH4-N, EC and ext-Na. Bacterial dynamics was profoundly influenced by NH4-N, EC and TC, with the decrease leading to discriminate genera shift from Sinibacillus and Thiopseudomonas to Brevbacterium, Brachybacterium, and Microbacterium. These findings suggest that mature compost was more desirable amendment than vegetable and food waste in the composting of NaOH/NaClO-contaminated poultry manure, and the decrease of ext-Na indicated compost maturity but did not influence bacterial dynamics.</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Brevibacterium</t>
+        </is>
+      </c>
+      <c r="C49" s="2" t="inlineStr">
+        <is>
+          <t>Liu, B., Li, Z., Yang, X., Du, C. &amp; Li, X. (2020). Microbiologically influenced corrosion of X80 pipeline steel by nitrate reducing bacteria in artificial Beijing soil.. Bioelectrochemistry (Amsterdam, Netherlands), 135, 107551.</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
+          <t>In this work, we investigated microbiologically influenced corrosion (MIC) of X80 pipeline steel caused by nitrate-reducing bacteria Brevibacterium frigoritolerans (B. frigoritolerans) in an artificial Beijing soil using electrochemical measurements and surface analyses under aerobic conditions. The B. frigoritolerans was isolated from the surrounding soil of the X80 pipeline steel specimen in Beijing using culturing and molecular biology techniques. Confocal laser scanning microscopy images showed that the largest pit depth after 14 days due to B. frigoritolerans was approximately 7.16 μm. Electrochemical tests showed that the B. frigoritolerans could change the stability of the corrosion products on the 7th day. Inhomogeneous biofilm and the conductivity of Fe&lt;sub&gt;2&lt;/sub&gt;O&lt;sub&gt;3&lt;/sub&gt; accelerated the corrosion process. The presence of NH&lt;sub&gt;4&lt;/sub&gt;&lt;sup&gt;+&lt;/sup&gt; on the surface of the X80 pipeline steel revealed that the B. frigoritolerans acted as a biological cathode to promote the cathodic reaction.</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Bulleidia</t>
+        </is>
+      </c>
+      <c r="C50" s="2" t="inlineStr">
+        <is>
+          <t>Jia, Y., et al. (2021). Association Between Oral Microbiota and Cigarette Smoking in the Chinese Population.. Frontiers in cellular and infection microbiology, 11, 658203.</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>The oral microbiota has been observed to be influenced by cigarette smoking and linked to several human diseases. However, research on the effect of cigarette smoking on the oral microbiota has not been systematically conducted in the Chinese population. We profiled the oral microbiota of 316 healthy subjects in the Chinese population by 16S rRNA gene sequencing. The alpha diversity of oral microbiota was different between never smokers and smokers (&lt;i&gt;P&lt;/i&gt; = 0.002). Several bacterial taxa were first reported to be associated with cigarette smoking by LEfSe analysis, including &lt;i&gt;Moryella&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 1.56E-04), &lt;i&gt;Bulleidia&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 1.65E-06), and &lt;i&gt;Moraxella&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 3.52E-02) at the genus level and &lt;i&gt;Rothia dentocariosa&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 1.55E-02), &lt;i&gt;Prevotella melaninogenica&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 8.48E-08), &lt;i&gt;Prevotella pallens&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 4.13E-03), &lt;i&gt;Bulleidia moorei&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 1.79E-06), &lt;i&gt;Rothia aeria&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 3.83E-06), &lt;i&gt;Actinobacillus parahaemolyticus&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 2.28E-04), and &lt;i&gt;Haemophilus parainfluenzae&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 4.82E-02) at the species level. Two nitrite-producing bacteria that can increase the acidity of the oral cavity, &lt;i&gt;Actinomyces&lt;/i&gt; and &lt;i&gt;Veillonella&lt;/i&gt;, were also enriched in smokers with FDR-adjusted &lt;i&gt;q&lt;/i&gt;-values of 3.62E-06 and 1.10E-06, respectively. Notably, we observed that two acid production-related pathways, amino acid-related enzymes (&lt;i&gt;q&lt;/i&gt; = 6.19E-05) and amino sugar and nucleotide sugar metabolism (&lt;i&gt;q&lt;/i&gt; = 2.63E-06), were increased in smokers by PICRUSt analysis. Finally, the co-occurrence analysis demonstrated that smoker-enriched bacteria were significantly positively associated with each other and were negatively correlated with the bacteria decreased in smokers. Our results suggested that cigarette smoking may affect oral health by creating a different environment by altering bacterial abundance, connections among oral microbiota, and the microbiota and their metabolic function.</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Cellulosimicrobium</t>
+        </is>
+      </c>
+      <c r="C51" s="2" t="inlineStr">
+        <is>
+          <t>Wyszkowska, J., Borowik, A., Zaborowska, M. &amp; Kucharski, J. (2022). Sensitivity of &lt;i&gt;Zea mays&lt;/i&gt; and Soil Microorganisms to the Toxic Effect of Chromium (VI).. International journal of molecular sciences, 24(1).</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>Chromium is used in many settings, and hence, it can easily enter the natural environment. It exists in several oxidation states. In soil, depending on its oxidation-reduction potential, it can occur in bivalent, trivalent or hexavalent forms. Hexavalent chromium compounds are cancerogenic to humans. The aim of this study was to determine the effect of Cr(VI) on the structure of bacteria and fungi in soil, to find out how this effect is modified by humic acids and to determine the response of &lt;i&gt;Zea mays&lt;/i&gt; to this form of chromium. A pot experiment was conducted to answer the above questions. &lt;i&gt;Zea mays&lt;/i&gt; was sown in natural soil and soil polluted with Cr(VI) in an amount of 60 mg kg&lt;sup&gt;-1&lt;/sup&gt; d.m. Both soils were treated with humic acids in the form of HumiAgra preparation. The ecophysiological and genetic diversity of bacteria and fungi was assayed in soil under maize (not sown with &lt;i&gt;Zea mays&lt;/i&gt;). In addition, the following were determined: yield of maize, greenness index, index of tolerance to chromium, translocation index and accumulation of chromium in the plant. It has been determined that Cr(VI) significantly distorts the growth and development of &lt;i&gt;Zea mays&lt;/i&gt;, while humic acids completely neutralize its toxic effect on the plant. This element had an adverse effect on the development of bacteria of the genera &lt;i&gt;Cellulosimicrobium&lt;/i&gt;, &lt;i&gt;Kaistobacter&lt;/i&gt;, &lt;i&gt;Rhodanobacter&lt;/i&gt;, &lt;i&gt;Rhodoplanes&lt;/i&gt; and &lt;i&gt;Nocardioides&lt;/i&gt; and fungi of the genera &lt;i&gt;Chaetomium and Humicola&lt;/i&gt;. Soil contamination with Cr(VI) significantly diminished the genetic diversity and richness of bacteria and the ecophysiological diversity of fungi. The negative impact of Cr(VI) on the diversity of bacteria and fungi was mollified by &lt;i&gt;Zea mays&lt;/i&gt; and the application of humic acids.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Clavibacter</t>
+        </is>
+      </c>
+      <c r="C52" s="2" t="inlineStr">
+        <is>
+          <t>Kaplan, M., et al. (2022). Investigation of Antibacterial Properties of Corrosion-Resistant 316L Steel Alloyed with 0.2 wt.% and 0.5 wt.% Ag.. Materials (Basel, Switzerland), 16(1).</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>The article is devoted to the study of melted ingots, plates rolled from them, and the resulting spherical powder made of corrosion-resistant 316L steel with the addition of 0.2 wt.% and 0.5 wt.% Ag. The study of antibacterial properties, microstructure, and distribution of silver concentrations, as well as qualitative analysis of silver content was carried out. The optimal mode of homogenization annealing of the ingot was 1050 °C for 9 h, which leads to the formation of an austenitic structure. It is shown that the addition of a small amount of silver does not affect the formation of the austenitic structure and silver is distributed evenly throughout the volume of the ingot. The austenitic structure also prevails in the plates after rolling. Silver is distributed evenly throughout the entire volume of the plate. It is noted that the addition of 0.2 wt.% Ag does not affect the strength, elongation, and microhardness of steel, and the addition of 0.5 wt.% Ag does not significantly reduce the strength of steel, however, all samples meet the mechanical characteristics according to the ASTM A240 standard. The qualitative chemical composition of samples made of corrosion-resistant steels was confirmed by X-ray fluorescence analysis methods. By the method of energy-dispersion analysis, the presence of a uniform distribution of silver over the entire volume of the powder particle was determined. The particles have a spherical shape with a minimum number of defects. The study of the antibacterial activity of plates and powder shows the presence of a clear antibacterial effect (bacteria of the genus Xanthomonas campestris, Erwinia carotovora, Pseudomonas marginalis, Clavibacter michiganensis) in samples No. 2 and No. 3 with the addition of 0.2 wt.% and 0.5 wt.% Ag.</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Clostridium</t>
+        </is>
+      </c>
+      <c r="C53" s="2" t="inlineStr">
+        <is>
+          <t>Ramos Monroy, O., Ruiz Ordaz, N., Hernández Gayosso, M., Juárez Ramírez, C. &amp; Galíndez Mayer, J. (2019). The corrosion process caused by the activity of the anaerobic sporulated bacterium Clostridium celerecrescens on API XL 52 steel.. Environmental science and pollution research international, 26(29), 29991-30002.</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>The microbial corrosion of oil and gas pipes is one of the problems occurring in the oil industry. Various mechanisms explaining microbial corrosion have been demonstrated. Commonly, biocorrosion is attributed to sulfate-reducing bacteria. Also, it has recently been reported that microbial species can connect their electron transport system to metal electrodes. In this research, two spore-forming bacteria isolated in different years from a gas pipeline were identified by biochemical techniques and by 16S rDNA amplification, sequencing, and comparison with the NCBI database. Isolates were also compared between them using molecular techniques as the restriction patterns, unique for 16S rDNA (ARDRA), and the profile of the amplified bit from the genomic DNA, using an unspecific primer (RAPD). The results obtained showed that both isolates corresponded to Clostridium celerecrescens with a 99% similarity according to the sequence reported on the NCBI database. Also, the ARDRA and RAPD electrophoretic profiles of both strains were identical, and no plasmids were found in the strains. Thus, it can be settled that this bacterium is persistent in the environment prevailing in gas pipelines. Also, it was demonstrated that the bacterial secretion of organic acids contributes to the pitting and general biocorrosion of API XL 52 steel. The rates of corrosion obtained, approximately after 40 days, were correlated with the presence and metabolic activity of C. celerecrescens on the metallic surfaces.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Cohnella</t>
+        </is>
+      </c>
+      <c r="C54" s="2" t="inlineStr">
+        <is>
+          <t>Shafiei, M., Afzali, F., Karkhane, A., Ebrahimi, S., Haghbeen, K. &amp; Aminzadeh, S. (2019). &lt;i&gt;Cohnella&lt;/i&gt; sp. A01 laccase: thermostable, detergent resistant, anti-environmental and industrial pollutants enzyme.. Heliyon, 5(9), e02543.</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>Laccase (EC 1.10.3.2; benzenediol; oxygen oxidoreductases) is a multi-copper oxidase that catalyzes the oxidation of phenols, polyphenols, aromatic amines, and different non-phenolic substrates with concomitant reduction of O&lt;sub&gt;2&lt;/sub&gt; to H&lt;sub&gt;2&lt;/sub&gt;O. Enzymatic oxidation techniques have the potential of implementation in different areas of industrial fields. In this study, the &lt;i&gt;Cohnella&lt;/i&gt; sp. A01 laccase gene was cloned into pET-26 (b+) vector and was transformed to &lt;i&gt;E. coli&lt;/i&gt; BL21. Then it was purified using His tag affinity (Ni sepharose resin) chromatography. The estimated molecular weight was approximately 60 kDa using SDS-PAGE. The highest enzyme activity and best pH for 2,6-dimethoxyphenol (DMP) oxidation were recorded as 8 at 90 °C respectively. The calculated half-life and kinetic values including K&lt;sub&gt;m&lt;/sub&gt;, V&lt;sub&gt;max&lt;/sub&gt;, turn over number (k&lt;sub&gt;cat&lt;/sub&gt;), and catalytic efficiency (k&lt;sub&gt;cat&lt;/sub&gt;/K&lt;sub&gt;m&lt;/sub&gt;) of the enzyme were 106 min at 90 °C and 686 μM, 10.69 U/ml, 20.3 S&lt;sup&gt;-&lt;/sup&gt;, and 0.029 s&lt;sup&gt;-1&lt;/sup&gt; μM&lt;sup&gt;-1&lt;/sup&gt;, respectively. The DMP was available as the substrate in all the calculations. Enzyme activity enhanced in the presence of Cu&lt;sup&gt;2+&lt;/sup&gt;, NaCl, SDS, n-hexane, Triton X-100, tween 20, and tween 80, significantly. The binding residues were predicted and mapped upon the modeled tertiary structure of identified laccase. The remaining activity and structural properties of &lt;i&gt;Cohnella&lt;/i&gt; sp. A01 laccase in extreme conditions such as high temperatures and presence of metals, detergents, and organic solvents suggest the potential of this enzyme in biotechnological and industrial applications. This process has been patented in Iranian Intellectual Property Centre under License No: 91325.</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Corynebacterium</t>
+        </is>
+      </c>
+      <c r="C55" s="2" t="inlineStr">
+        <is>
+          <t>Zhang, D., et al. (2024). The relationships of metals exposure and disturbance of the vaginal microbiota with the risk of PROM: Results from a birth cohort study.. Ecotoxicology and environmental safety, 289, 117420.</t>
+        </is>
+      </c>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>The vaginal microbiota is proposed to be associated with reproductive health. Exposure to metals during pregnancy is a risk factor for premature rupture of membranes (PROM). PROM can lead to serious maternal complications, thus, identifying the cause and therapeutic targets for it is crucial. However, the role of vaginal microbiota in the association between metals exposure and the risk of PROM are not clear. Based on a prospective birth cohort study including 668 pregnant women, maternal blood levels of 15 metals in the first trimester (n=668) and microbiota of vaginal secretions in the third trimester (n=244) were assessed. The metals that significantly associated with the risk of PROM were screened out via four statistical models, the top three were barium (Ba), chromium (Cr) and thallium (Tl) according to their weight indices. The results from the BKMR model showed a positive association of the mixture (Ba, Cr and Tl) with the risk of PROM. PROM and non-PROM were characterised by different beta diversities, moreover, the relative abundances of Bifidobacterium, Corynebacterium and Collinsella were statistically and negatively related to the risk of PROM [the adjusted odds ratios (ORs) and 95 % confidence intervals (CIs) were 0.06 (0.00, 0.82), 0.32 (0.14, 0.74) and 0.50 (0.30, 0.84), respectively]. On the other hand, women with different levels of Ba exposure were also characterised by different beta diversities (p value = 0.047); and blood Ba levels were also negatively associated with the relative abundances of Collinsella; additionally, Cr levels were positively associated with alpha diversity indices [Shannon index: β (95 % CI) = 0.25 (0.01, 0.50); Simpson index: β (95 % CI) = 0.08 (0.00, 0.17), respectively]. The results from mediation analysis showed the proportion of the relationship between Ba exposure and PROM risk mediated by the relative abundance of Collinsella was 26.4 %. Further verification analysis exploring the potential cause of the above phenomenon indicated that the neutrophil count, one of blood inflammation indicators for PROM, was higher in women with the absence of Collinsella (p value = 0.039), moreover, the cumulative hazard of PROM for women with the presence of Collinsella was also significantly lower than that of those without Collinsella (p value = 0.007). Collectively, the changes in the diversity and composition of the bacterial community, especially the reduction in Collinsella abundance caused by metal exposure, may be related to the occurrence of PROM, which provides a new microbiota-based perspective for intervention in metal exposure-related PROM. Confirming these relationships and determining the possible processes at play will require more investigation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Enterococcus</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="inlineStr">
+        <is>
+          <t>Conforte, J., Sousa, C., da Silva, A., Ribeiro, A., Duque, C. &amp; Assunção, W. (2023). Effect of &lt;i&gt;Enterococcus faecalis&lt;/i&gt; Biofilm on Corrosion Kinetics in Titanium Grade 4 Alloys with Different Surface Treatments.. Materials (Basel, Switzerland), 16(13).</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>&lt;i&gt;E. faecalis&lt;/i&gt; has been associated with bacteremia, sepsis, and bacterial endocarditis and peri-implantitis. This microorganism can remain in the alveolus even after extraction of the root remnant. This study aimed to evaluate the corrosion on different surfaces of commercially pure titanium (Ti) grade 4 (Ticp-G4) as a function of the bacterial biofilm effect of &lt;i&gt;Enterococcus faecalis&lt;/i&gt;. A total of 57 discs were randomly divided according to their surface finish (n = 19). For microbiological analysis (n = 9), the discs were placed in 12-well plates containing &lt;i&gt;E. faecalis&lt;/i&gt; culture and incubated at 37 °C for 7 days. The results show that for the intergroup analysis, considering the "electrolyte" factor, there was a difference between the groups. There was greater biofilm formation for the D.A.Zir group, with greater electrochemical exchange for Biofilm, and the presence of biofilm favored greater electrochemical exchange with the medium.</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>354</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Halomonas</t>
+        </is>
+      </c>
+      <c r="C57" s="2" t="inlineStr">
+        <is>
+          <t>Li, C., et al. (2024). Effect of Halomonas titanicae on fluctuating water-line corrosion of EH40 steel.. Bioelectrochemistry (Amsterdam, Netherlands), 158, 108703.</t>
+        </is>
+      </c>
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>The fluctuating water-line corrosion of EH40 steel in sterile and biotic media was investigated with a wire beam electrode. When the coupons were partially immersed in the sterile medium, the position of the low water-line acted as the cathodic zone and the area below the low water-line constantly served as the main anodic zone. The thin electrolyte layers with uneven thickness promoted the galvanic current of the region below the low water-line. Different from the sterile environment, the metabolism of Halomonas titanica with oxygen as the final electron acceptor reduced the dissolved oxygen concentration, which resulted in the position of the low water-line acting as the anodic zone.</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>408</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Legionella</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="inlineStr">
+        <is>
+          <t>Spencer-Williams, I., Meyer, M., DePas, W., Elliott, E. &amp; Haig, S. (2023). Assessing the Impacts of Lead Corrosion Control on the Microbial Ecology and Abundance of Drinking-Water-Associated Pathogens in a Full-Scale Drinking Water Distribution System.. Environmental science &amp; technology, 57(48), 20360-20369.</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>Increases in phosphate availability in drinking water distribution systems (DWDSs) from the use of phosphate-based corrosion control strategies may result in nutrient and microbial community composition shifts in the DWDS. This study assessed the year-long impacts of full-scale DWDS orthophosphate addition on both the microbial ecology and density of drinking-water-associated pathogens that infect the immunocompromised (DWPIs). Using 16S rRNA gene amplicon sequencing and droplet digital PCR, drinking water microbial community composition and DWPI density were examined. Microbial community composition analysis suggested significant compositional changes after the orthophosphate addition. Significant increases in total bacterial density were observed after orthophosphate addition, likely driven by a 2 log 10 increase in nontuberculous mycobacteria (NTM). Linear effect models confirmed the importance of phosphate addition with phosphorus concentration explaining 17% and 12% of the variance in NTM and &lt;i&gt;L. pneumophila&lt;/i&gt; density, respectively. To elucidate the impact of phosphate on NTM aggregation, a comparison of planktonic and aggregate fractions of NTM cultures grown at varying phosphate concentrations was conducted. Aggregation assay results suggested that higher phosphate concentrations cause more disaggregation, and the interaction between phosphate and NTM is species specific. This work reveals new insight into the consequences of orthophosphate application on the DWDS microbiome and highlights the importance of proactively monitoring the DWDS for DWPIs.</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>456</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Methyloversatilis</t>
+        </is>
+      </c>
+      <c r="C59" s="2" t="inlineStr">
+        <is>
+          <t>Shrestha, R., et al. (2021). Anaerobic microbial corrosion of carbon steel under conditions relevant for deep geological repository of nuclear waste.. The Science of the total environment, 800, 149539.</t>
+        </is>
+      </c>
+      <c r="D59" s="2" t="inlineStr">
+        <is>
+          <t>We examined microbial corrosion of carbon steel in synthetic bentonite pore water inoculated with natural underground water containing microorganisms over a period of 780-days under sterile and anaerobic conditions. Corrosion behaviour was determined using the mass loss method, SEM-EDS analysis and Raman spectroscopy, while qualitative and quantitative changes in the microbial community were analysed using molecular-biological tools (16S rDNA amplicon sequencing and qPCR analysis, respectively). Corrosion rates were significantly higher in the biotic environment (compared with an abiotic environment), with significant localisation of corrosion attacks of up to 1 mm arising within 12-months. Nitrate reducing bacteria, such as Pseudomonas, Brevundimonas and Methyloversatilis, dominated the microbial consortium, the high abundance of Methyloversatilis correlating with periods of highest localised corrosion penetrations, suggesting that this bacterium plays an important role in microbially influenced corrosion. Our results indicate that nitrate-reducing bacteria could represent a potential threat to waste canisters under nuclear repository conditions.</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>470</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Mycobacterium</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="inlineStr">
+        <is>
+          <t>Song, Y., et al. (2019). Distinct microbially induced concrete corrosion at the tidal region of reinforced concrete sewers.. Water research, 150, 392-402.</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>Microbially induced concrete corrosion (MICC) is a major deterioration affecting sewers worldwide. MICC is not uniform on sewer inner walls and often occurs at hot spots such as crown and tidal regions, which are critical to determine sewer service life. Especially, concrete corrosion in tidal regions is complicated due to the fluctuation of wastewater levels and the hydraulic scouring effects. The traditional methodology of corrosion monitoring also limits the study of the tidal corrosion. In this study, by using a combination of various advanced mineral analytical techniques and culture-independent 16S rRNA gene amplicon sequencing, the development of corrosion, the formation of corrosion products and the variation of microbial communities in tidal regions were investigated systematically. The physical-chemical characteristics in tidal regions varied with the distance from the wastewater surface. Above the wastewater, more severe corrosion was detected with a closer distance to wastewater, producing gypsum as the major corrosion products. The microbial succession in tidal regions occurred, with the coexistence of conventional autotrophic SOB and acidophilic heterotrophic bacteria initially, and shifting to the predominant colonization of Mycobacterium when pH reached around 1. The heterotrophic bacteria, i.e. Mycobacterium and Bacillus, were likely responsible for the observed corrosion due to the potential capability in generating sulfuric acid. The applications of advanced mineral and microbial analytical techniques were demonstrated effective in improving the understanding of concrete sewer corrosion.</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>471</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Mycoplana</t>
+        </is>
+      </c>
+      <c r="C61" s="2" t="inlineStr">
+        <is>
+          <t>Sabri, N., Zakaria, Z., Mohamad, S., Jaafar, A. &amp; Hara, H. (2018). Importance of Soil Temperature for the Growth of Temperate Crops under a Tropical Climate and Functional Role of Soil Microbial Diversity.. Microbes and environments, 33(2), 144-150.</t>
+        </is>
+      </c>
+      <c r="D61" s="2" t="inlineStr">
+        <is>
+          <t>A soil cooling system that prepares soil for temperate soil temperatures for the growth of temperate crops under a tropical climate is described herein. Temperate agriculture has been threatened by the negative impact of temperature increases caused by climate change. Soil temperature closely correlates with the growth of temperate crops, and affects plant processes and soil microbial diversity. The present study focuses on the effects of soil temperatures on lettuce growth and soil microbial diversity that maintains the growth of lettuce at low soil temperatures. A model temperate crop, loose leaf lettuce, was grown on eutrophic soil under soil cooling and a number of parameters, such as fresh weight, height, the number of leaves, and root length, were evaluated upon harvest. Under soil cooling, significant differences were observed in the average fresh weight (P&lt;0.05) and positive development of the roots, shoots, and leaves of lettuce. Janthinobacterium (8.142%), Rhodoplanes (1.991%), Arthrospira (1.138%), Flavobacterium (0.857%), Sphingomonas (0.790%), Mycoplana (0.726%), and Pseudomonas (0.688%) were the dominant bacterial genera present in cooled soil. Key soil fungal communities, including Pseudaleuria (18.307%), Phoma (9.968%), Eocronartium (3.527%), Trichosporon (1.791%), and Pyrenochaeta (0.171%), were also recovered from cooled soil. The present results demonstrate that the growth of temperate crops is dependent on soil temperature, which subsequently affects the abundance and diversity of soil microbial communities that maintain the growth of temperate crops at low soil temperatures.</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>474</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Neisseria</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="inlineStr">
+        <is>
+          <t>Henriksen, S. (1974). "Pitting" and "corrosion" of the surface of agar cultures by colonies of some bacteria from the respiratory tract.. Acta pathologica et microbiologica Scandinavica. Section B: Microbiology and immunology, 82(1), 48-52.</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>491</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Novosphingobium</t>
+        </is>
+      </c>
+      <c r="C63" s="2" t="inlineStr">
+        <is>
+          <t>Ju, Y., et al. (2024). Evaluating radionuclide mobility in groundwater recharge areas of fractured natural barrier systems using multiple isotopes and microbial indicators.. Journal of hazardous materials, 482, 136571.</t>
+        </is>
+      </c>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>The distribution of uranium (U) concentrations, which reached up to 322 µg/L, was found to correlate with the pattern of fractures within the natural barrier system (NBS). Analysis of the vertical distribution of dissolved oxygen (DO), dissolved organic carbon (DOC), tritium (&lt;sup&gt;3&lt;/sup&gt;H), microbial communities, and H&lt;sub&gt;2&lt;/sub&gt;O and SO&lt;sub&gt;4&lt;/sub&gt;&lt;sup&gt;2-&lt;/sup&gt; isotopes revealed insights into oxic water infiltration within the heterogeneous fractured system. Their distribution showed that the average infiltration depth at the KURT site is 200 m, while in external areas with a high frequency of fractures, oxic conditions extended down to 495 m. The SO&lt;sub&gt;4&lt;/sub&gt;&lt;sup&gt;2-&lt;/sup&gt; isotopes suggested the potential for microbial sulfate reduction to play a role in regulating radionuclide mobility in the deep geological system. At approximately 500 m, genera capable of thriving under harsh conditions of low DO and high heavy metal concentrations, such as Novosphingobium, Comamonadaceae_uc, and Desulfuromonas_g2, were identified. These findings indicate hydrogeological variability and microbial adaptation within the deep NBS, highlighting the importance of understanding the deep geological environment for evaluating microbiome performance in regulating toxic radionuclides within repository systems. Overall, this study emphasizes the pivotal role of age tracers, stable isotopes, and microbiome in enhancing the assessment of the long-term stability of fractured granite barriers.</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>497</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Oerskovia</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="inlineStr">
+        <is>
+          <t>Rana, S., Kumar, A., Walia, S., Berven, K., Cumper, K. &amp; Walia, S. (2011). Isolation of Tn1546-like elements in vancomycin-resistant Enterococcus faecium isolated from wood frogs: an emerging risk for zoonotic bacterial infections to humans.. Journal of applied microbiology, 110(1), 35-43.</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>Isolation and characterization of vancomycin-resistant enterococci (VRE), mainly Enterococcus faecium, from the faecal pellet of wood frogs (Rana sylvatica).</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>503</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Opitutus</t>
+        </is>
+      </c>
+      <c r="C65" s="2" t="inlineStr">
+        <is>
+          <t>Quan, L., et al. (2024). Rice husk biochar is more effective in blocking the cadmium and lead accumulation in two Brassica vegetables grown on a contaminated field than sugarcane bagasse biochar.. Environmental geochemistry and health, 46(11), 471.</t>
+        </is>
+      </c>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>Heavy metal-contaminated soil has a great impact on yield reduction of vegetable crops and soil microbial community destruction. Biochar-derived waste biomass is one of the most commonly applied soil conditioners in heavy metal-contaminated soil. Different heavy metal-contaminated soil added with suitable biochars represent an intriguing way of the safe production of crops. This study investigated the effects of two types of biochar [rice husk biochar (RHB) and sugarcane bagasse biochar (SBB)] on Cd and Pb accumulation in Shanghaiqing (SHQ, a variety of Brassica campestris L.) and Fengyou 737 (FY, a variety of Brassica napus), as well as on the soil microbial community, through a field experiment. RHB and SBB were characterized by scanning electron microscopy, Fourier transform infrared spectroscopy, and Brunauer-Emmet-Teller method. The results showed that RHB and SBB displayed the higher pH, cation exchange capacity and pore properties, and the addition of RHB and SBB enhanced soil pH and rhizosphere microorganisms promoting vegetables yield. RHB treatments were more effective than SBB in reducing upward transfer of Cd and Pb, blocking the accumulation of Cd and Pb in the edible parts of SHQ and FY, and decreasing soil Cd and Pb bioavailability. Additionally, RHB and SBB changed the composition of the rhizosphere soil microbial community. The application of biochar promoted the growth of ecologically beneficial bacteria (Nitrospira, Opitutus, and Gemmatimonas) and fungi (Mortierella and Holtermanniella), whereas reducing the enrichment of plant pathogenic fungi (Alternaria, Stagonosporopsis, Lectera, and Periconia) in rhizosphere soil. Our findings demonstrated that the application of RHB significantly reduces Cd and Pb accumulation in the edible parts by decreasing the soil Cd and Pb bioavailability and altering the rhizosphere microbial community composition in two Brassica vegetables grown on Cd/Pb-contaminated soils. Thus, the application of two biochar, especially RHB is a feasible strategy for the safe production of vegetable crops in Cd/Pb co-contaminated soils.</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>512</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Oxobacter</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="inlineStr"/>
+      <c r="D66" s="2" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>526</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Paracoccus</t>
+        </is>
+      </c>
+      <c r="C67" s="2" t="inlineStr">
+        <is>
+          <t>Huber, B., Drewes, J., Lin, K., König, R. &amp; Müller, E. (2014). Revealing biogenic sulfuric acid corrosion in sludge digesters: detection of sulfur-oxidizing bacteria within full-scale digesters.. Water science and technology : a journal of the International Association on Water Pollution Research, 70(8), 1405-11.</t>
+        </is>
+      </c>
+      <c r="D67" s="2" t="inlineStr">
+        <is>
+          <t>Biogenic sulfuric acid corrosion (BSA) is a costly problem affecting both sewerage infrastructure and sludge handling facilities such as digesters. The aim of this study was to verify BSA in full-scale digesters by identifying the microorganisms involved in the concrete corrosion process, that is, sulfate-reducing (SRB) and sulfur-oxidizing bacteria (SOB). To investigate the SRB and SOB communities, digester sludge and biofilm samples were collected. SRB diversity within digester sludge was studied by applying polymerase chain reaction-denaturing gradient gel electrophoresis (PCR-DGGE) targeting the dsrB-gene (dissimilatory sulfite reductase beta subunit). To reveal SOB diversity, cultivation dependent and independent techniques were applied. The SRB diversity studies revealed different uncultured SRB, confirming SRB activity and H2S production. Comparable DGGE profiles were obtained from the different sludges, demonstrating the presence of similar SRB species. By cultivation, three pure SOB strains from the digester headspace were obtained including Acidithiobacillus thiooxidans, Thiomonas intermedia and Thiomonas perometabolis. These organisms were also detected with PCR-DGGE in addition to two new SOB: Thiobacillus thioparus and Paracoccus solventivorans. The SRB and SOB responsible for BSA were identified within five different digesters, demonstrating that BSA is a problem occurring not only in sewer systems but also in sludge digesters. In addition, the presence of different SOB species was successfully associated with the progression of microbial corrosion.</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>566</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Prevotella</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="inlineStr">
+        <is>
+          <t>Fagunwa, O., Davies, K. &amp; Bradbury, J. (2024). The Human Gut and Dietary Salt: The &lt;i&gt;Bacteroides&lt;/i&gt;/&lt;i&gt;Prevotella&lt;/i&gt; Ratio as a Potential Marker of Sodium Intake and Beyond.. Nutrients, 16(7).</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="inlineStr">
+        <is>
+          <t>The gut microbiota is a dynamic ecosystem that plays a pivotal role in maintaining host health. The perturbation of these microbes has been linked to several health conditions. Hence, they have emerged as promising targets for understanding and promoting good health. Despite the growing body of research on the role of sodium in health, its effects on the human gut microbiome remain under-explored. Here, using nutrition and metagenomics methods, we investigate the influence of dietary sodium intake and alterations of the human gut microbiota. We found that a high-sodium diet (HSD) altered the gut microbiota composition with a significant reduction in &lt;i&gt;Bacteroides&lt;/i&gt; and inverse increase in &lt;i&gt;Prevotella&lt;/i&gt; compared to a low-sodium diet (LSD). However, there is no clear distinction in the Firmicutes/Bacteroidetes (F/B) ratio between the two diet types. Metabolic pathway reconstruction revealed the presence of sodium reabsorption genes in the HSD, but not LSD. Since it is currently difficult in microbiome studies to confidently associate the F/B ratio with what is considered healthy (e.g., low sodium) or unhealthy (e.g., high sodium), we suggest that the use of a genus-based ratio such as the &lt;i&gt;Bacteroides&lt;/i&gt;/&lt;i&gt;Prevotella&lt;/i&gt; (B/P) ratio may be more beneficial for the application of microbiome studies in health.</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>581</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Psb-m-3</t>
+        </is>
+      </c>
+      <c r="C69" s="2" t="inlineStr">
+        <is>
+          <t>Pei, Y., Yu, Z., Ji, J., Khan, A. &amp; Li, X. (2018). Microbial Community Structure and Function Indicate the Severity of Chromium Contamination of the Yellow River.. Frontiers in microbiology, 9, 38.</t>
+        </is>
+      </c>
+      <c r="D69" s="2" t="inlineStr">
+        <is>
+          <t>The Yellow River is the most important water resource in northern China. In the recent past, heavy metal contamination has become severe due to industrial processes and other anthropogenic activities. In this study, riparian soil samples with varying levels of chromium (Cr) pollution severity were collected along the Gansu industrial reach of the Yellow River, including samples from uncontaminated sites (XC, XGU), slightly contaminated sites (LJX, XGD), and heavily contaminated sites (CG, XG). The Cr concentrations of these samples varied from 83.83 mg⋅kg&lt;sup&gt;-1&lt;/sup&gt; (XGU) to 506.58 mg⋅kg&lt;sup&gt;-1&lt;/sup&gt; (XG). The chromate [Cr (VI)] reducing ability in the soils collected in this study followed the sequence of the heavily contaminated &gt; slightly contaminated &gt; the un-contaminated. Common Cr remediation genes &lt;i&gt;chrA&lt;/i&gt; and &lt;i&gt;yieF&lt;/i&gt; were detected in the XG and CG samples. qRT-PCR results showed that the expression of &lt;i&gt;chrA&lt;/i&gt; was up-regulated four and threefold in XG and CG samples, respectively, whereas the expression of &lt;i&gt;yieF&lt;/i&gt; was up-regulated 66- and 7-fold in the same samples after 30 min treatment with Cr (VI). The copy numbers of &lt;i&gt;chrA&lt;/i&gt; and &lt;i&gt;yieF&lt;/i&gt; didn't change after 35 days incubation with Cr (VI). The microbial communities in the Cr contaminated sampling sites were different from those in the uncontaminated samples. Especially, the relative abundances of &lt;i&gt;Firmicutes&lt;/i&gt; and &lt;i&gt;Bacteroidetes&lt;/i&gt; were higher while &lt;i&gt;Actinobacteria&lt;/i&gt; was lower in the contaminated group than uncontaminated group. Further, potential indicator species, related to Cr such as Cr-remediation genera (&lt;i&gt;Geobacter, PSB-M-3, Flavobacterium&lt;/i&gt;, and &lt;i&gt;Methanosarcina&lt;/i&gt;); the Cr-sensitive genera (&lt;i&gt;Skermanella, Iamia, Arthrobacter&lt;/i&gt;, and &lt;i&gt;Candidatus Nitrososphaera&lt;/i&gt;) were also identified. These data revealed that Cr shifted microbial composition and function. Further, Cr (VI) reducing ability could be related with the expression of Cr remediation genes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>583</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Pseudarthrobacter</t>
+        </is>
+      </c>
+      <c r="C70" s="2" t="inlineStr">
+        <is>
+          <t>Luo, Y., et al. (2024). Penicillium oxalicum SL2-enhanced nanoscale zero-valent iron effectively reduces Cr(VI) and shifts soil microbiota.. Journal of hazardous materials, 469, 134058.</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>Most current researches focus solely on reducing soil chromium availability. It is difficult to reduce soil Cr(VI) concentration below 5.0 mg kg&lt;sup&gt;-1&lt;/sup&gt; using single remediation technology. This study introduced a sustainable soil Cr(VI) reduction and stabilization system, Penicillium oxalicum SL2-nanoscale zero-valent iron (nZVI), and investigated its effect on Cr(VI) reduction efficiency and microbial ecology. Results showed that P. oxalicum SL2-nZVI effectively reduced soil total Cr(VI) concentration from 187.1 to 3.4 mg kg&lt;sup&gt;-1&lt;/sup&gt; within 180 d, and remained relatively stable at 360 d. The growth curve of P. oxalicum SL2 and microbial community results indicated that γ-ray irradiation shortened the adaptation time of P. oxalicum SL2 and facilitated its colonization in soil. P. oxalicum SL2 colonization activated nZVI and its derivatives, and increased soil iron bioavailability. After restoration, the negative effect of Cr(VI) on soil microorganisms was markedly alleviated. Cr(VI), Fe(II), bioavailable Cr/Fe, Eh, EC and urease (SUE) were the key environmental factors of soil microbiota. Notably, Penicillium significantly stimulated the growth of urease-positive bacteria, Arthrobacter, Pseudarthrobacter, and Microvirga, synergistically reducing soil chromium availability. The combination of P. oxalicum SL2 and nZVI is expected to form a green, economical and long-lasting Cr(VI) reduction stabilization strategy.</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>584</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Pseudoalteromonas</t>
+        </is>
+      </c>
+      <c r="C71" s="2" t="inlineStr">
+        <is>
+          <t>Liang, Y., Wang, P. &amp; Zhang, D. (2021). Designing a Highly Stable Slippery Organogel on Q235 Carbon Steel for Inhibiting Microbiologically Influenced Corrosion.. ACS applied bio materials, 4(8), 6056-6064.</t>
+        </is>
+      </c>
+      <c r="D71" s="2" t="inlineStr">
+        <is>
+          <t>Microbiologically influenced corrosion (MIC) accelerates the corrosion and degradation of metal materials due to the settlement of microorganisms on the surface. However, environmentally friendly and efficient methods to fabricate antifouling and anticorrosion surfaces are still lacking. Inspired by &lt;i&gt;Nepenthes&lt;/i&gt;, a slippery liquid-infused porous surface (SLIPS) has been proven to be an efficient way to inhibit settlement of microorganisms on the metal surface and the following MIC due to the existence of a mobile defect-free lubricant layer. However, the stability of the lubricant layer and substrate of the SLIPS prevented its long-term antifouling and anticorrosion application. Herein, a highly stable slippery organogel was fabricated by depositing a homogeneous mixture of PDMS (base and curing agent), silicone oil, triethoxyvinylsilane, and SiO&lt;sub&gt;2&lt;/sub&gt; on Q235 and curing in an oven. Triethoxyvinylsilane was not only able to cross-link with the curing agent of PDMS through hydrosilylation but also able to interlink the organogel and Q235 through condensation between the -OH of the metal surface and hydrolyzed siloxane. As a result, the adhesion force between the organogel without triethoxyvinylsilane and the substrate (0.45 MPa) increased to 1.50 MPa for the organogel with triethoxyvinylsilane and SiO&lt;sub&gt;2&lt;/sub&gt;. Also, the tensile strength of the organogel without SiO&lt;sub&gt;2&lt;/sub&gt; (0.97 MPa) increased to 3.88 MPa for the organogel with 2 wt % SiO&lt;sub&gt;2&lt;/sub&gt; because of the high elastic modulus of SiO&lt;sub&gt;2&lt;/sub&gt;, which was important to improving its stability under external force. In addition, the organogel showed stable oil distribution and slippery performance after spinning at 4000 rpm for 30 s. Then, the bacterial settlement demonstrated that the organogel could effectively inhibit &lt;i&gt;Pseudoalteromonas&lt;/i&gt; sp. settlement on the substrate under both static and dynamic conditions. Finally, an electrochemical test indicated that the MIC could be effectively mitigated by the organogel. This study provides an efficient method to fabricate a highly stable slippery surface on a metal surface for its potential application in mitigating MIC.</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>621</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Roseateles</t>
+        </is>
+      </c>
+      <c r="C72" s="2" t="inlineStr">
+        <is>
+          <t>Muthukumarasamy, R., Revathi, G., Vadivelu, M. &amp; Arun, K. (2017). Isolation of bacterial strains possessing nitrogen-fixation, phosphate and potassium-solubilization and their inoculation effects on sugarcane.. Indian journal of experimental biology, 55(3), 161-70.</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="inlineStr">
+        <is>
+          <t>Inorganic nitrogen (N), phosphate (P) and potash (K) are the most influencing macro-nutrients for plant growth and microbial supplementation of these minerals through N2-fixation, P- and K-solubilization is gaining importance. In the present study, a macronutrient deficient (MD), N-free novel medium, supplemented with tri calcium phosphate (TCP as P- source) and Mica (as K- source) was used for isolation of microbes possessing nitrogen fixing, P- &amp; K solubilizing abilities. Samples of rhizosphere and non-rhizosphere soils, roots and leaves of sugarcane varieties (viz., Co 6304, Co 86032 and CoC 671) collected from Tamil Nadu, India were used for isolation. Totally, 8 individual nitrogen-fixing, phosphate- and potash-solubilizing bacterial strains were obtained. Nitrogen-fixing abilities of these isolates were confirmed by analyzing acetylene reduction (AR) activity and the presence of nif genes. P- and K- solubilizing activities were confirmed by cultivating these isolates in solid/liquid medium supplemented with insoluble forms of P and K. These isolates which produced growth hormone IAA, were in two groups as Roseateles terrae and Burkholderia gladioli, respectively based on the morphological, physiological, biochemical and 16S rDNA gene sequence analysis. Association between diazotrophic, P- and K-solubilizing R. terrae and B. gladioli with sugarcane has not been reported earlier. These isolates were tested for their growth-promoting abilities in sugarcane cultivated in pots, and the results showed that these isolates were able to increase the leaf chlorophyll, N content and total biomass. This study may encourage farmers to use single microbe for microbial supplementation of N, P and K instead of consortium of microbes wherein the compatibility between different microbes is often compromised.</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>687</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Streptococcus</t>
+        </is>
+      </c>
+      <c r="C73" s="2" t="inlineStr">
+        <is>
+          <t>Yang, C., et al. (2021). Corrosion behavior of high nitrogen nickel-free austenitic stainless steel in the presence of artificial saliva and Streptococcus mutans.. Bioelectrochemistry (Amsterdam, Netherlands), 142, 107940.</t>
+        </is>
+      </c>
+      <c r="D73" s="2" t="inlineStr">
+        <is>
+          <t>High nitrogen nickel-free austenitic stainless steels (HNSs) have great potentials to be used in dentistry owing to its exceptional mechanical properties, high corrosion resistance, and biocompatibility. In this study, HNSs with nitrogen of 0.88 wt% and 1.08 wt% displayed much lower maximum pit depths than 316L stainless steel (SS) after 21 d of immersion in abiotic artificial saliva (2.2 μm and 1.7 μm vs. 4.5 μm). Microbiologically influenced corrosion (MIC) evaluations revealed that Streptococcus mutans biofilms led to much severer corrosion of 316L SS than HNSs. Corrosion current densities of HNSs were two orders of magnitude lower than that of 316L SS after incubation of 7 d (37.5 nA/cm&lt;sup&gt;2&lt;/sup&gt; and 29.9 nA/cm&lt;sup&gt;2&lt;/sup&gt; vs. 5.63 μA/cm&lt;sup&gt;2&lt;/sup&gt;). The pitting potentials of HNSs were at least 550 mV higher than that of 316L SS in the presence of S. mutans, confirming the better MIC resistance of HNSs. Cytotoxicity assay confirmed that HNSs were not toxic to MC3T3-E1 cells and allowed better sessile cell growth on them than on 316L SS. It can be concluded that HNSs are more suitable dental materials than the conventional 316L SS.</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>727</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Thiobacillus</t>
+        </is>
+      </c>
+      <c r="C74" s="2" t="inlineStr">
+        <is>
+          <t>Dubey, R. &amp; Upadhyay, S. (2001). Microbial corrosion monitoring by an amperometric microbial biosensor developed using whole cell of Pseudomonas sp.. Biosensors &amp; bioelectronics, 16(9-12), 995-1000.</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="inlineStr">
+        <is>
+          <t>A microbial biosensor was developed for monitoring microbiologically influenced corrosion (MIC) of metallic materials in industrial systems. The Pseudomonas sp. isolated from corroded metal surface was immobilized on acetylcellulose membrane and its respiratory activity was estimated by measuring oxygen consumption. The microbial biosensor was used for the measurement of sulfuric acid in a batch culture medium contaminated by microorganisms. A linear relationship between the microbial sensor response and the concentration of sulfuric acid was observed. The response time of biosensor was 5 min and was dependent on the immobilized cell loading of Pseudomonas sp., pH, temperature and corrosive environments. The microbial biosensor response was stable, reproducible and specific for sensing of sulfur oxidizing bacterial activity.</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0</v>
+      </c>
+      <c r="C75" s="2" t="inlineStr">
+        <is>
+          <t>Su, Y., et al. (2024). Facile and green synthesis of Ag/Cu bimetallic nanoparticles using waste banana peel extract for effective corrosion inhibition of mixed sulfate-reducing bacteria.. Journal of environmental management, 373, 123713.</t>
+        </is>
+      </c>
+      <c r="D75" s="2" t="inlineStr">
+        <is>
+          <t>Microbiologically induced corrosion (MIC) is widespread in the oilfield industry, and new environmentally friendly materials are urgently needed to inhibit MIC with the increasing environmental requirements and microbial resistance problems. The synthesis method and cost of the materials are important factors that must be considered in the production and application. In this study, Ag/Cu bimetallic nanoparticles (BNPs) were synthesized by eco-friendly and sustainable method using waste banana peel extract (BPE) as a green reducing. The antibacterial and corrosion inhibition properties of Ag/Cu BNPs were investigated by using the enriched mixed strains containing sulfate-reducing bacteria (SRB) as model bacteria. The results of electron microscopy showed that the prepared BNPs exhibited spherical structure with about 19.0 nm in size. The synthesized nanoparticles significantly inhibited the growth of mixed strains by antimicrobial experiments with minimum inhibitory concentration (MIC) value of 9.38 μg/mL. The addition of Ag/Cu BNPs (9.38 μg/mL) inhibited the corrosion of X65 carbon steel induced by the mixed strains with 77.9% compared to the untreated condition. Correspondingly, the number of sessile SRB cells in the solution containing Ag/Cu BNPs (9.38 μg/mL) after 28 days of immersion decreased by 5-log compared with the treatment group without nanomaterials (1.1 × 10&lt;sup&gt;8&lt;/sup&gt; cells/cm&lt;sup&gt;2&lt;/sup&gt;). Furthermore, the observation of the surface morphology and strains cellular microstructure of carbon steel treated with nanoparticle materials illustrated that the corrosion inhibition mechanism mainly includes destroying cell structure, affecting metabolic activities and inhibiting biofilm formation. The environmentally friendly nanoparticle materials prepared in this study have great potential in the safe and clean production of oil fields.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Consolidating sequences with iTOL tree
</commit_message>
<xml_diff>
--- a/data_Ref/bacteria_corrosion_summary_improved.xlsx
+++ b/data_Ref/bacteria_corrosion_summary_improved.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2389,6 +2389,1124 @@
       <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr"/>
     </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Actinomyces</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation; sulfate_reduction; acid_production</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>186.4</v>
+      </c>
+      <c r="E76" t="n">
+        <v>492</v>
+      </c>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Anaerococcus</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E77" t="n">
+        <v>11</v>
+      </c>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr"/>
+      <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Aquabacter</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr"/>
+      <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Aquabacterium</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="E79" t="n">
+        <v>18</v>
+      </c>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr"/>
+      <c r="J79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Atopobium</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>biofilm_formation; sulfate_reduction; metal_reduction; acid_production</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="E80" t="n">
+        <v>27</v>
+      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Cellulosimicrobium</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="E81" t="n">
+        <v>9</v>
+      </c>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Clostridium</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>636.1</v>
+      </c>
+      <c r="E82" t="n">
+        <v>1905</v>
+      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr"/>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Colwellia</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>18.1</v>
+      </c>
+      <c r="E83" t="n">
+        <v>18</v>
+      </c>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr"/>
+      <c r="H83" t="inlineStr"/>
+      <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Corynebacterium</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>215.5</v>
+      </c>
+      <c r="E84" t="n">
+        <v>609</v>
+      </c>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr"/>
+      <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>334</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Gelria</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>metal_reduction; acid_production</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="E85" t="n">
+        <v>1</v>
+      </c>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr"/>
+      <c r="H85" t="inlineStr"/>
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>342</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Georgfuchsia</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>metal_reduction; acid_production; biofilm_formation; sulfate_reduction</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="E86" t="n">
+        <v>3</v>
+      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr"/>
+      <c r="I86" t="inlineStr"/>
+      <c r="J86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>351</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Haemophilus</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>571.3000000000001</v>
+      </c>
+      <c r="E87" t="n">
+        <v>1825</v>
+      </c>
+      <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr"/>
+      <c r="I87" t="inlineStr"/>
+      <c r="J87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>426</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Lyngbya</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>metal_reduction; acid_production; sulfate_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>9.699999999999999</v>
+      </c>
+      <c r="E88" t="n">
+        <v>11</v>
+      </c>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr"/>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>471</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Mycoplana</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E89" t="n">
+        <v>1</v>
+      </c>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>480</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Nitratireductor</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E90" t="n">
+        <v>4</v>
+      </c>
+      <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr"/>
+      <c r="J90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>494</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Oceaniovalibus</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" t="inlineStr"/>
+      <c r="G91" t="inlineStr"/>
+      <c r="H91" t="inlineStr"/>
+      <c r="I91" t="inlineStr"/>
+      <c r="J91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>541</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Peptoclostridium</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>metal_reduction; acid_production</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>2</v>
+      </c>
+      <c r="E92" t="n">
+        <v>2</v>
+      </c>
+      <c r="F92" t="inlineStr"/>
+      <c r="G92" t="inlineStr"/>
+      <c r="H92" t="inlineStr"/>
+      <c r="I92" t="inlineStr"/>
+      <c r="J92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>549</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Phenylobacterium</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>3</v>
+      </c>
+      <c r="E93" t="n">
+        <v>3</v>
+      </c>
+      <c r="F93" t="inlineStr"/>
+      <c r="G93" t="inlineStr"/>
+      <c r="H93" t="inlineStr"/>
+      <c r="I93" t="inlineStr"/>
+      <c r="J93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>565</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Porphyromonas</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>344.8</v>
+      </c>
+      <c r="E94" t="n">
+        <v>1033</v>
+      </c>
+      <c r="F94" t="inlineStr"/>
+      <c r="G94" t="inlineStr"/>
+      <c r="H94" t="inlineStr"/>
+      <c r="I94" t="inlineStr"/>
+      <c r="J94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>584</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Pseudoalteromonas</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>69.39999999999999</v>
+      </c>
+      <c r="E95" t="n">
+        <v>129</v>
+      </c>
+      <c r="F95" t="inlineStr"/>
+      <c r="G95" t="inlineStr"/>
+      <c r="H95" t="inlineStr"/>
+      <c r="I95" t="inlineStr"/>
+      <c r="J95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>605</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Rhodanobacter</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="E96" t="n">
+        <v>27</v>
+      </c>
+      <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr"/>
+      <c r="I96" t="inlineStr"/>
+      <c r="J96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>625</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Roseococcus</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>metal_reduction</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>1</v>
+      </c>
+      <c r="E97" t="n">
+        <v>1</v>
+      </c>
+      <c r="F97" t="inlineStr"/>
+      <c r="G97" t="inlineStr"/>
+      <c r="H97" t="inlineStr"/>
+      <c r="I97" t="inlineStr"/>
+      <c r="J97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>636</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Ruminococcaceae_ucg-005</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>sulfate_reduction</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="E98" t="n">
+        <v>2</v>
+      </c>
+      <c r="F98" t="inlineStr"/>
+      <c r="G98" t="inlineStr"/>
+      <c r="H98" t="inlineStr"/>
+      <c r="I98" t="inlineStr"/>
+      <c r="J98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>657</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Shinella</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="E99" t="n">
+        <v>8</v>
+      </c>
+      <c r="F99" t="inlineStr"/>
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>678</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Sphingosinicella</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
+      <c r="F100" t="inlineStr"/>
+      <c r="G100" t="inlineStr"/>
+      <c r="H100" t="inlineStr"/>
+      <c r="I100" t="inlineStr"/>
+      <c r="J100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>712</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Tepidimonas</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E101" t="n">
+        <v>2</v>
+      </c>
+      <c r="F101" t="inlineStr"/>
+      <c r="G101" t="inlineStr"/>
+      <c r="H101" t="inlineStr"/>
+      <c r="I101" t="inlineStr"/>
+      <c r="J101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>725</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Thermus</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>74.09999999999999</v>
+      </c>
+      <c r="E102" t="n">
+        <v>178</v>
+      </c>
+      <c r="F102" t="inlineStr"/>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr"/>
+      <c r="I102" t="inlineStr"/>
+      <c r="J102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>864</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Veillonella</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation; sulfate_reduction; acid_production</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>88.3</v>
+      </c>
+      <c r="E103" t="n">
+        <v>191</v>
+      </c>
+      <c r="F103" t="inlineStr"/>
+      <c r="G103" t="inlineStr"/>
+      <c r="H103" t="inlineStr"/>
+      <c r="I103" t="inlineStr"/>
+      <c r="J103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>871</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Xanthobacter</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation; sulfate_reduction</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>11.7</v>
+      </c>
+      <c r="E104" t="n">
+        <v>15</v>
+      </c>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr"/>
+      <c r="H104" t="inlineStr"/>
+      <c r="I104" t="inlineStr"/>
+      <c r="J104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>872</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Xanthomonadaceae_bacterium_wwh73</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>biofilm_formation; sulfate_reduction</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>2</v>
+      </c>
+      <c r="E105" t="n">
+        <v>2</v>
+      </c>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="inlineStr"/>
+      <c r="H105" t="inlineStr"/>
+      <c r="I105" t="inlineStr"/>
+      <c r="J105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Azospira</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="E106" t="n">
+        <v>25</v>
+      </c>
+      <c r="F106" t="inlineStr"/>
+      <c r="G106" t="inlineStr"/>
+      <c r="H106" t="inlineStr"/>
+      <c r="I106" t="inlineStr"/>
+      <c r="J106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Brachybacterium</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="E107" t="n">
+        <v>6</v>
+      </c>
+      <c r="F107" t="inlineStr"/>
+      <c r="G107" t="inlineStr"/>
+      <c r="H107" t="inlineStr"/>
+      <c r="I107" t="inlineStr"/>
+      <c r="J107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Bulleidia</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>metal_reduction</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>1</v>
+      </c>
+      <c r="E108" t="n">
+        <v>1</v>
+      </c>
+      <c r="F108" t="inlineStr"/>
+      <c r="G108" t="inlineStr"/>
+      <c r="H108" t="inlineStr"/>
+      <c r="I108" t="inlineStr"/>
+      <c r="J108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Cellulosimicrobium</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="E109" t="n">
+        <v>9</v>
+      </c>
+      <c r="F109" t="inlineStr"/>
+      <c r="G109" t="inlineStr"/>
+      <c r="H109" t="inlineStr"/>
+      <c r="I109" t="inlineStr"/>
+      <c r="J109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Clostridium</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>sulfate_reduction; metal_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>636.1</v>
+      </c>
+      <c r="E110" t="n">
+        <v>1905</v>
+      </c>
+      <c r="F110" t="inlineStr"/>
+      <c r="G110" t="inlineStr"/>
+      <c r="H110" t="inlineStr"/>
+      <c r="I110" t="inlineStr"/>
+      <c r="J110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Corynebacterium</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>215.5</v>
+      </c>
+      <c r="E111" t="n">
+        <v>609</v>
+      </c>
+      <c r="F111" t="inlineStr"/>
+      <c r="G111" t="inlineStr"/>
+      <c r="H111" t="inlineStr"/>
+      <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>354</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Halomonas</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation; sulfate_reduction; acid_production</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="E112" t="n">
+        <v>91</v>
+      </c>
+      <c r="F112" t="inlineStr"/>
+      <c r="G112" t="inlineStr"/>
+      <c r="H112" t="inlineStr"/>
+      <c r="I112" t="inlineStr"/>
+      <c r="J112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>408</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Legionella</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction; biofilm_formation</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>165</v>
+      </c>
+      <c r="E113" t="n">
+        <v>396</v>
+      </c>
+      <c r="F113" t="inlineStr"/>
+      <c r="G113" t="inlineStr"/>
+      <c r="H113" t="inlineStr"/>
+      <c r="I113" t="inlineStr"/>
+      <c r="J113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>471</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Mycoplana</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr"/>
+      <c r="D114" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E114" t="n">
+        <v>1</v>
+      </c>
+      <c r="F114" t="inlineStr"/>
+      <c r="G114" t="inlineStr"/>
+      <c r="H114" t="inlineStr"/>
+      <c r="I114" t="inlineStr"/>
+      <c r="J114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>497</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Oerskovia</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E115" t="n">
+        <v>1</v>
+      </c>
+      <c r="F115" t="inlineStr"/>
+      <c r="G115" t="inlineStr"/>
+      <c r="H115" t="inlineStr"/>
+      <c r="I115" t="inlineStr"/>
+      <c r="J115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>512</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Oxobacter</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr"/>
+      <c r="D116" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0</v>
+      </c>
+      <c r="F116" t="inlineStr"/>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" t="inlineStr"/>
+      <c r="I116" t="inlineStr"/>
+      <c r="J116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>526</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Paracoccus</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>metal_reduction; biofilm_formation; sulfate_reduction; acid_production</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>121.6</v>
+      </c>
+      <c r="E117" t="n">
+        <v>298</v>
+      </c>
+      <c r="F117" t="inlineStr"/>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" t="inlineStr"/>
+      <c r="I117" t="inlineStr"/>
+      <c r="J117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>581</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Psb-m-3</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>metal_reduction</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>1</v>
+      </c>
+      <c r="E118" t="n">
+        <v>1</v>
+      </c>
+      <c r="F118" t="inlineStr"/>
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" t="inlineStr"/>
+      <c r="I118" t="inlineStr"/>
+      <c r="J118" t="inlineStr"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t>584</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Pseudoalteromonas</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>metal_reduction; sulfate_reduction; biofilm_formation; acid_production</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>69.39999999999999</v>
+      </c>
+      <c r="E119" t="n">
+        <v>129</v>
+      </c>
+      <c r="F119" t="inlineStr"/>
+      <c r="G119" t="inlineStr"/>
+      <c r="H119" t="inlineStr"/>
+      <c r="I119" t="inlineStr"/>
+      <c r="J119" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2400,7 +3518,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3828,6 +4946,856 @@
         </is>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Actinomyces</t>
+        </is>
+      </c>
+      <c r="C76" s="2" t="inlineStr">
+        <is>
+          <t>Zhang, Y., et al. (2015). Tantalum Nitride-Decorated Titanium with Enhanced Resistance to Microbiologically Induced Corrosion and Mechanical Property for Dental Application.. PloS one, 10(6), e0130774.</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="inlineStr">
+        <is>
+          <t>Microbiologically induced corrosion (MIC) of metallic devices/implants in the oral region is one major cause of implant failure and metal allergy in patients. Therefore, it is crucial to develop practical approaches which can effectively prevent MIC for broad clinical applications of these materials. In the present work, tantalum nitride (TaN)-decorated titanium with promoted bio-corrosion and mechanical property was firstly developed via depositing TaN layer onto pure Ti using magnetron sputtering. The microstructure and chemical constituent of TaN coatings were characterized, and were found to consist of a hard fcc-TaN outer layer. Besides, the addition of TaN coatings greatly increased the hardness and modulus of pristine Ti from 2.54 ± 0.20 to 29.88 ± 2.59 GPa, and from 107.19 ± 6.98 to 295.46 ± 19.36 GPa, respectively. Potentiodynamic polarization and electrochemical impedance spectroscopy studies indicated that TaN coating exhibited higher MIC resistance in comparison to bare Ti and TiN-coated coating in two bacteria-containing artificial saliva solutions. Moreover, the biofilm experiment showed that the TaN-decorated Ti sample possessed good antibacterial performance. The SEM and XPS results after biofilm removal demonstrated that TaN film remained its integrity and stability, while TiN layer detached from Ti surface in the bio-corrosion tests, demonstrating the anti-MIC behavior and the strong binding property of TaN coating to Ti substrate. Considering all these results, TaN-decorated Ti material exhibits the optimal comprehensive performance and holds great potential as implant material for dental applications.</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Anaerococcus</t>
+        </is>
+      </c>
+      <c r="C77" s="2" t="inlineStr">
+        <is>
+          <t>Akgül, Ö., Söyletir, G. &amp; Ülger Toprak, N. (2020). [Antimicrobial Susceptibility of Pathogenic Gram-positive Anaerobic Cocci: Data of a University Hospital in Turkey].. Mikrobiyoloji bulteni, 54(3), 404-417.</t>
+        </is>
+      </c>
+      <c r="D77" s="2" t="inlineStr">
+        <is>
+          <t>Gram-positive anaerobic cocci (GPAC), a large group of anaerobic bacteria, are the members of the normal microbiota that colonizes the skin and mucosal surfaces of the human body. However, in case of a wound or when the host becomes immunocompromised, GPAC can cause invasive and most frequently mixed infections. GPAC are the second most frequently isolated bacteria in anaerobic infections. Although the studies are limited, GPAC have been reported to develop resistance to antimicrobial drugs. The resistance of the pathogens to the antimicrobials and improper therapy can cause poor clinical outcomes. Therefore, monitoring of the resistance trends of regional clinically important anaerobic bacteria periodically is recommended. In our study, we aimed to determine the antimicrobial susceptibility profiles of clinically important GPAC. A total of 100 non-duplicated pathogenic GPAC isolates were collected from Marmara University Hospital between 2013 and 2015. The isolates were identified by using conventional methods, "matrix-assisted laser desorption ionization-time of flight mass spectrometry system (MALDI-TOF MS)" (VITEK MS; v3.0, bioMerieux, France) and 16S rRNA gene sequencing. Antimicrobial susceptibility test was carried out by the agar dilution method according to the Clinical and Laboratory Standards Institute (CLSI) guidelines. The following antimicrobials were tested: penicillin, amoxicillin/ clavulanic acid (AMC), cefoxitin, meropenem, clindamycin, erythromycin, tetracycline, tigecycline, chloramphenicol, moxifloxacin and metronidazole. The minimum inhibitory concentration (MIC) results were interpreted according to the breakpoints described by the European Committee on Antimicrobial Susceptibility Testing (EUCAST). Breakpoints recommended by CLSI for cefoxitin, tetracycline and moxifloxacin, and breakpoint recommended by Food and Drug Administration (FDA) for tigecycline were used since there were no EUCAST breakpoints for these antimicrobials. MIC50 and MIC90 values were determined for erythromycin since the breakpoint was not described by EUCAST, CLSI or FDA guidelines. The identification results showed that the strains (n= 100) consisted of five different GPAC genus; Parvomonas (40%), Finegoldia (34%), Peptoniphilus (14%), Peptostreptococcus (10%) and Anaerococcus (1%). All of the organisms were susceptible to meropenem, tigecycline and metronidazole. The isolates were highly susceptible to penicillin, AMC, cefoxitin, and chloramphenicol, since the resistance rates against these antimicrobials were 5% or less. The resistance rates against clindamycin, tetracycline and moxifloxacin were 14%, 31% and 24%, respectively. In total, 11% of the isolates were multidrug resistant. Metronidazole and tigecycline displayed high in vitro activity against GPAC and both are appropriate antimicrobials for the selection of empiric therapy. The effectiveness of meropenem was also found high, but it was observed that this antimicrobial would be more appropriate to use in the treatment of severe mixed infections accompanied by other microorganisms with the resistance potential. Detection of penicillin and AMC resistant isolates, which are frequently used in the treatment of GPAC infection, requires periodic monitoring of the antimicrobial susceptibility patterns of GPAC. The high rates of resistance against clindamycin, tetracycline and moksifloxacin indicated that these antimicrobials should not be used for empirical treatment of infections without prior antimicrobial susceptibility testing. This study is one of the largest susceptibility studies specifically carried out on GPAC to date in Turkey. We believe that our results will provide good surveillance data both for our hospital and our country.</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Aquabacter</t>
+        </is>
+      </c>
+      <c r="C78" s="2" t="inlineStr"/>
+      <c r="D78" s="2" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Aquabacterium</t>
+        </is>
+      </c>
+      <c r="C79" s="2" t="inlineStr">
+        <is>
+          <t>Jin, J., Wu, G. &amp; Guan, Y. (2015). Effect of bacterial communities on the formation of cast iron corrosion tubercles in reclaimed water.. Water research, 71, 207-18.</t>
+        </is>
+      </c>
+      <c r="D79" s="2" t="inlineStr">
+        <is>
+          <t>To understand the role bacterial communities play in corrosion scale development, the morphological and physicochemical characteristics of corrosion scales in raw and disinfected reclaimed water were systematically investigated. Corrosion tubercles were found in raw reclaimed water while thin corrosion layers formed in disinfected reclaimed water. The corrosion tubercles, composed mainly of α-FeOOH, γ-FeOOH, and CaCO3, consisted of an top surface; a shell containing more magnetite than other layers; a core in association with stalks produced by bacteria; and a corroded layer. The thin corrosion layers also had layered structures. These had a smooth top, a dense middle, and a corroded layer. They mostly consisted of the same main components as the tubercles in raw reclaimed water, but with different proportions. The profiles of the dissolved oxygen (DO) concentration, redox potential, and pH in the tubercles were different to those in the corrosion layers, which demonstrated that these parameters changed with a shift in the microbial processes in the tubercles. The bacterial communities in the tubercles were found to be dominated by Proteobacteria (56.7%), Bacteroidetes (10.0%), and Nitrospira (6.9%). The abundance of sequences affiliated to iron-reducing bacteria (IRB, mainly Geothrix) and iron-oxidizing bacteria (mainly Aquabacterium) was relatively high. The layered characteristics of the corrosion layers was due to the blocking of DO transfer by the development of the scales themselves. Bacterial communities could at least promote the layering process and formation of corrosion tubercles. Possible mechanisms might include: (1) bacterial communities mediated the pH and redox potential in the tubercles (which helped to form shell-like and core layers), (2) the metabolism of IRB and magnetic bacteria (Magnetospirillum) might contribute to the presence of Fe3O4 in the shell-like layer, while IRB contributed to green rust in the core layer, and (3) the diversity of the bacterial community resulted in the complex composition of the core layer, and gas producing bacteria (sulfate-reducing bacteria and methanogenic bacteria) played a role in the formation of the porous core layer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Atopobium</t>
+        </is>
+      </c>
+      <c r="C80" s="2" t="inlineStr">
+        <is>
+          <t>Marcas, J., Romero, L., Tipiani, O., Loyola, S. &amp; Tamariz, J. (2022). In vitro antimicrobial activity of Bixa orellana L . Leaves extract against anaerobic bacteria associated to bacterial vaginosis and Lactobacillus spp.. Revista peruana de medicina experimental y salud publica, 39(4), 408-414.</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="inlineStr">
+        <is>
+          <t>Motivation for the study: bacterial vaginosis is a bacterial infection that frequently affects women of reproductive age. The treatment is based on synthetic antimicrobials. Bixa orellana L. possesses antimicrobial properties and could represent a potential non-synthetic therapeutic alternative. Main findings: in vitro results suggest that, methanolic extract of Bixa orellana L. leaves possesses potential antimicrobial properties against bacteria associated to bacterial vaginosis. Implications: to identify new sources with therapeutic potential, and to promote research, discovery, and characterization of non-synthetic antimicrobials. To describe the in vitro antimicrobial activity of the methanolic extract of Bixa orellana L. leaves against anaerobic bacteria associated to bacterial vaginosis and Lactobacillus spp.</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Cellulosimicrobium</t>
+        </is>
+      </c>
+      <c r="C81" s="2" t="inlineStr">
+        <is>
+          <t>Wyszkowska, J., Borowik, A., Zaborowska, M. &amp; Kucharski, J. (2022). Sensitivity of &lt;i&gt;Zea mays&lt;/i&gt; and Soil Microorganisms to the Toxic Effect of Chromium (VI).. International journal of molecular sciences, 24(1).</t>
+        </is>
+      </c>
+      <c r="D81" s="2" t="inlineStr">
+        <is>
+          <t>Chromium is used in many settings, and hence, it can easily enter the natural environment. It exists in several oxidation states. In soil, depending on its oxidation-reduction potential, it can occur in bivalent, trivalent or hexavalent forms. Hexavalent chromium compounds are cancerogenic to humans. The aim of this study was to determine the effect of Cr(VI) on the structure of bacteria and fungi in soil, to find out how this effect is modified by humic acids and to determine the response of &lt;i&gt;Zea mays&lt;/i&gt; to this form of chromium. A pot experiment was conducted to answer the above questions. &lt;i&gt;Zea mays&lt;/i&gt; was sown in natural soil and soil polluted with Cr(VI) in an amount of 60 mg kg&lt;sup&gt;-1&lt;/sup&gt; d.m. Both soils were treated with humic acids in the form of HumiAgra preparation. The ecophysiological and genetic diversity of bacteria and fungi was assayed in soil under maize (not sown with &lt;i&gt;Zea mays&lt;/i&gt;). In addition, the following were determined: yield of maize, greenness index, index of tolerance to chromium, translocation index and accumulation of chromium in the plant. It has been determined that Cr(VI) significantly distorts the growth and development of &lt;i&gt;Zea mays&lt;/i&gt;, while humic acids completely neutralize its toxic effect on the plant. This element had an adverse effect on the development of bacteria of the genera &lt;i&gt;Cellulosimicrobium&lt;/i&gt;, &lt;i&gt;Kaistobacter&lt;/i&gt;, &lt;i&gt;Rhodanobacter&lt;/i&gt;, &lt;i&gt;Rhodoplanes&lt;/i&gt; and &lt;i&gt;Nocardioides&lt;/i&gt; and fungi of the genera &lt;i&gt;Chaetomium and Humicola&lt;/i&gt;. Soil contamination with Cr(VI) significantly diminished the genetic diversity and richness of bacteria and the ecophysiological diversity of fungi. The negative impact of Cr(VI) on the diversity of bacteria and fungi was mollified by &lt;i&gt;Zea mays&lt;/i&gt; and the application of humic acids.</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Clostridium</t>
+        </is>
+      </c>
+      <c r="C82" s="2" t="inlineStr">
+        <is>
+          <t>Ramos Monroy, O., Ruiz Ordaz, N., Hernández Gayosso, M., Juárez Ramírez, C. &amp; Galíndez Mayer, J. (2019). The corrosion process caused by the activity of the anaerobic sporulated bacterium Clostridium celerecrescens on API XL 52 steel.. Environmental science and pollution research international, 26(29), 29991-30002.</t>
+        </is>
+      </c>
+      <c r="D82" s="2" t="inlineStr">
+        <is>
+          <t>The microbial corrosion of oil and gas pipes is one of the problems occurring in the oil industry. Various mechanisms explaining microbial corrosion have been demonstrated. Commonly, biocorrosion is attributed to sulfate-reducing bacteria. Also, it has recently been reported that microbial species can connect their electron transport system to metal electrodes. In this research, two spore-forming bacteria isolated in different years from a gas pipeline were identified by biochemical techniques and by 16S rDNA amplification, sequencing, and comparison with the NCBI database. Isolates were also compared between them using molecular techniques as the restriction patterns, unique for 16S rDNA (ARDRA), and the profile of the amplified bit from the genomic DNA, using an unspecific primer (RAPD). The results obtained showed that both isolates corresponded to Clostridium celerecrescens with a 99% similarity according to the sequence reported on the NCBI database. Also, the ARDRA and RAPD electrophoretic profiles of both strains were identical, and no plasmids were found in the strains. Thus, it can be settled that this bacterium is persistent in the environment prevailing in gas pipelines. Also, it was demonstrated that the bacterial secretion of organic acids contributes to the pitting and general biocorrosion of API XL 52 steel. The rates of corrosion obtained, approximately after 40 days, were correlated with the presence and metabolic activity of C. celerecrescens on the metallic surfaces.</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Colwellia</t>
+        </is>
+      </c>
+      <c r="C83" s="2" t="inlineStr">
+        <is>
+          <t>Shibulal, B., Smith, M., Cooper, I., Burgess, H., Moles, N. &amp; Willows, A. (2024). Deciphering microbial communities involved in marine steel corrosion using high-throughput amplicon sequencing.. Environmental microbiology reports, 16(4), e70001.</t>
+        </is>
+      </c>
+      <c r="D83" s="2" t="inlineStr">
+        <is>
+          <t>To characterize the source and effects of bacterial communities on corrosion of intertidal structures, three different UK coastal sites were sampled for corrosion materials, sediment and seawater. Chemical analyses indicate the activity of sulfate-reducing microbes (SRBs) at 2 sites (Shoreham and Newhaven), but not at the third (Southend-on-Sea). Microbial communities in the deep sediment and corrosion samples are similar. The phylum Proteobacteria is dominant (40.4% of the total ASV), followed by Campilobacterota (11.3%), Desulfobacterota and Firmicutes (4%-5%). At lower taxonomic levels, corrosion causing bacteria, such as Shewanella sp. (6%), Colwellia sp. (7%) and Mariprofundus sp. (1%), are present. At Southend-on-sea, the relative abundance of Campilobacterota is higher compared to the other two sites. The mechanism of action of microorganisms at Shoreham and Newhaven involves biogenic sulfuric acid corrosion of iron by the combined action of SRBs and sulfur-oxidizing microbes. However, at Southend-on-sea, sulfur compounds are not implicated in corrosion, but SRBs and other electroactive microbes may play a role in which cathodic reactions (electrical MIC) and microbial enzymes (chemical MIC) are involved. To contribute to diagnosis of accelerated intertidal corrosion types, we developed a rapid identification method for SRBs using quantitative polymerase chain reaction high-resolution melt curve analysis of the dsrB gene.</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Corynebacterium</t>
+        </is>
+      </c>
+      <c r="C84" s="2" t="inlineStr">
+        <is>
+          <t>Zhang, D., et al. (2024). The relationships of metals exposure and disturbance of the vaginal microbiota with the risk of PROM: Results from a birth cohort study.. Ecotoxicology and environmental safety, 289, 117420.</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="inlineStr">
+        <is>
+          <t>The vaginal microbiota is proposed to be associated with reproductive health. Exposure to metals during pregnancy is a risk factor for premature rupture of membranes (PROM). PROM can lead to serious maternal complications, thus, identifying the cause and therapeutic targets for it is crucial. However, the role of vaginal microbiota in the association between metals exposure and the risk of PROM are not clear. Based on a prospective birth cohort study including 668 pregnant women, maternal blood levels of 15 metals in the first trimester (n=668) and microbiota of vaginal secretions in the third trimester (n=244) were assessed. The metals that significantly associated with the risk of PROM were screened out via four statistical models, the top three were barium (Ba), chromium (Cr) and thallium (Tl) according to their weight indices. The results from the BKMR model showed a positive association of the mixture (Ba, Cr and Tl) with the risk of PROM. PROM and non-PROM were characterised by different beta diversities, moreover, the relative abundances of Bifidobacterium, Corynebacterium and Collinsella were statistically and negatively related to the risk of PROM [the adjusted odds ratios (ORs) and 95 % confidence intervals (CIs) were 0.06 (0.00, 0.82), 0.32 (0.14, 0.74) and 0.50 (0.30, 0.84), respectively]. On the other hand, women with different levels of Ba exposure were also characterised by different beta diversities (p value = 0.047); and blood Ba levels were also negatively associated with the relative abundances of Collinsella; additionally, Cr levels were positively associated with alpha diversity indices [Shannon index: β (95 % CI) = 0.25 (0.01, 0.50); Simpson index: β (95 % CI) = 0.08 (0.00, 0.17), respectively]. The results from mediation analysis showed the proportion of the relationship between Ba exposure and PROM risk mediated by the relative abundance of Collinsella was 26.4 %. Further verification analysis exploring the potential cause of the above phenomenon indicated that the neutrophil count, one of blood inflammation indicators for PROM, was higher in women with the absence of Collinsella (p value = 0.039), moreover, the cumulative hazard of PROM for women with the presence of Collinsella was also significantly lower than that of those without Collinsella (p value = 0.007). Collectively, the changes in the diversity and composition of the bacterial community, especially the reduction in Collinsella abundance caused by metal exposure, may be related to the occurrence of PROM, which provides a new microbiota-based perspective for intervention in metal exposure-related PROM. Confirming these relationships and determining the possible processes at play will require more investigation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>334</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Gelria</t>
+        </is>
+      </c>
+      <c r="C85" s="2" t="inlineStr">
+        <is>
+          <t>Kim, E., Lee, J., Han, G. &amp; Hwang, S. (2018). Comprehensive analysis of microbial communities in full-scale mesophilic and thermophilic anaerobic digesters treating food waste-recycling wastewater.. Bioresource technology, 259, 442-450.</t>
+        </is>
+      </c>
+      <c r="D85" s="2" t="inlineStr">
+        <is>
+          <t>Microbes were sampled for a year in a full-scale mesophilic anaerobic digester (MD) and a thermophilic anaerobic digester (TD) treating food waste-recycling wastewater (FRW), then microbial community structure, dynamics and diversity were quantified. In the MD, Fastidiosipila, Petrimonas, vadinBC27, Syntrophomonas, and Proteiniphilum were dominant bacterial genera; they may contribute to hydrolysis and fermentation. In the TD, Defluviitoga, Gelria and Tepidimicrobium were dominant bacteria; they may be responsible for hydrolysis and acid production. In the MD, dominant methanogens changed from Methanobacterium (17.1 ± 16.9%) to Methanoculleus (67.7 ± 17.8%) due to the increase in ammonium concentration. In the TD, dominant methanogens changed from Methanoculleus (42.8 ± 13.6%) to Methanothermobacter (49.6 ± 11.0%) due to the increase of pH. Bacteria and archaea were more diverse in the MD than in the TD. These results will guide development of microbial management methods to improve the process stability of MD and TD treating FRW.</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>342</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Georgfuchsia</t>
+        </is>
+      </c>
+      <c r="C86" s="2" t="inlineStr">
+        <is>
+          <t>Atashgahi, S., et al. (2021). Proteogenomic analysis of Georgfuchsia toluolica revealed unexpected concurrent aerobic and anaerobic toluene degradation.. Environmental microbiology reports, 13(6), 841-851.</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="inlineStr">
+        <is>
+          <t>Denitrifying Betaproteobacteria play a key role in the anaerobic degradation of monoaromatic hydrocarbons. We performed a multi-omics study to better understand the metabolism of the representative organism Georgfuchsia toluolica strain G5G6 known as a strict anaerobe coupling toluene oxidation with dissimilatory nitrate and Fe(III) reduction. Despite the genomic potential for degradation of different carbon sources, we did not find sugar or organic acid transporters, in line with the inability of strain G5G6 to use these substrates. Using a proteomics analysis, we detected proteins of fumarate-dependent toluene activation, membrane-bound nitrate reductase, and key components of the metal-reducing (Mtr) pathway under both nitrate- and Fe(III)-reducing conditions. High abundance of the multiheme cytochrome MtrC implied that a porin-cytochrome complex was used for respiratory Fe(III) reduction. Remarkably, strain G5G6 contains a full set of genes for aerobic toluene degradation, and we detected enzymes of aerobic toluene degradation under both nitrate- and Fe(III)-reducing conditions. We further detected an ATP-dependent benzoyl-CoA reductase, reactive oxygen species detoxification proteins, and cytochrome c oxidase indicating a facultative anaerobic lifestyle of strain G5G6. Correspondingly, we found diffusion through the septa a substantial source of oxygen in the cultures enabling concurrent aerobic and anaerobic toluene degradation by strain G5G6.</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>351</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Haemophilus</t>
+        </is>
+      </c>
+      <c r="C87" s="2" t="inlineStr">
+        <is>
+          <t>Faisal, S., Ullah, R., Alotaibi, A., Zafar, S., Rizwan, M. &amp; Tariq, M. (2023). Biofabrication of silver nanoparticles employing biomolecules of Paraclostridium benzoelyticum strain: Its characterization and their in-vitro antibacterial, anti-aging, anti-cancer and other biomedical applications.. Microscopy research and technique, 86(7), 846-861.</t>
+        </is>
+      </c>
+      <c r="D87" s="2" t="inlineStr">
+        <is>
+          <t>The current study aims to utilize the bacteria Paraclostridium benzoelyticum strain 5610 to synthesize bio-genic silver nanoparticles (AgNPs). Biogenic AgNPs were thoroughly examined using various characterization techniques such as UV-spectroscopy, XRD, FTIR, SEM, and EDX. Synthesis of AgNPs was confirmed by UV-vis analysis resulting in absorption peak at 448.31 nm wavelength. The SEM analysis indicated the morphological characteristics and size of AgNPs which was 25.29 nm. The face centered cubic (FCC) crystallographic structure was confirmed by XRD. Furthermore, FTIR study affirmed the capping of AgNPs by different compounds found in biomass of the Paraclostridium benzoelyticum strain 5610. Later, EDX was used to determine the elemental composition with respective concentration and distribution. Additionally, in the current study the antibacterial, anti-inflammatory, antioxidant, anti-aging, and anti-cancer ability of AgNPs was assessed. The antibacterial activity of AgNPs was tested against four distinct sinusitis pathogens: Haemophilus in-fluenza, Streptococcus pyogenes, Moraxella catarrhalis and Streptococcus pneumonia. AgNPs shows significant inhibition zone against Streptococcus pyogenes 16.64 ± 0.35 followed by 14.32 ± 071 for Moraxella catarrhalis. Similarly, the antioxidant potential was found maximum (68.37 ± 0.55%) at 400 μg/mL and decrease (5.48 ± 0.65%) at 25 μg/mL, hence the significant antioxidant ability was observed. Furthermore, anti-inflammatory activity of AgNPs shows the strongest inhibitory action (42.68 ± 0.62%) for 15-LOX with lowest inhibition activity for COX-2 (13.16 ± 0.46%). AgNPs have been shown to exhibit significant inhibitory actions against the enzyme elastases AGEs (66.25 ± 0.49%), which are followed by AGEs of visperlysine (63.27 ± 0.69%). Furthermore, the AgNPs show high toxicity against HepG2 cell line which shows 53.543% reduction in the cell viability after 24 h of treatment. The anti-inflammatory activity demonstrated a potent inhibitory effect of the bio-inspired AgNPs. Overall, the biogenic AgNPs have the ability to be served for the treatments of anti-aging and also due to their anti-cancer, antioxidant abilities NPs may be a useful therapy choice for a variety of disorders including cancer, bacterial infections and other inflammatory diseases. Moreover, further studies are required in the future to evaluate their in vivo biomedical applications. HIGHLIGHTS: Biogenic synthesis of AgNPs using Paraclostridium benzoelyticum Strain for the first time. FTIR analysis confirmed capping of potent biomolecules which are of great use in applied field especially Nanomedicines. Notable antimicrobial activity against sinusitis bacteria and cytotoxic potential of synthesized AgNPs on in vitro basis produce a new idea shifting us to treat cancerous cell lines.</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>426</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Lyngbya</t>
+        </is>
+      </c>
+      <c r="C88" s="2" t="inlineStr">
+        <is>
+          <t>Parvin, N., Mandal, S. &amp; Rath, J. (2024). Microbiome of seventh-century old Parsurameswara stone monument of India and role of desiccation-tolerant cyanobacterium &lt;i&gt;Lyngbya corticicola&lt;/i&gt; on its biodeterioration.. Biofouling, 40(1), 40-53.</t>
+        </is>
+      </c>
+      <c r="D88" s="2" t="inlineStr">
+        <is>
+          <t>The Parsurameswara stone monument, built in the seventh century, is one of the oldest stone monuments in Odisha, India. Metagenomic analysis of the biological crust samples collected from the stone monument revealed 17 phyla in the microbiome, with Proteobacteria being the most dominant phylum, followed by cyanobacteria. Eight cyanobacteria were isolated. &lt;i&gt;Lyngbya corticicola&lt;/i&gt; was the dominant cyanobacterium in all crust samples and could tolerate six months of desiccation &lt;i&gt;in vitro&lt;/i&gt;. With six months of desiccation, chlorophyll-&lt;i&gt;a&lt;/i&gt; decreased; however, carotenoid and cellular carbohydrate contents of this organism increased in the desiccated state. Resistance to desiccation, high carotenoid content, and effective trehalose biosynthesis in this cyanobacterium provide a distinct advantage over other microbiomes. Comparative metabolic profiles of the biological crust and &lt;i&gt;L. corticicola&lt;/i&gt; show strongly corrosive organic acids such as dichloroacetic acid, which might be responsible for the biocorrosion of stone monuments.</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>471</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Mycoplana</t>
+        </is>
+      </c>
+      <c r="C89" s="2" t="inlineStr">
+        <is>
+          <t>Sabri, N., Zakaria, Z., Mohamad, S., Jaafar, A. &amp; Hara, H. (2018). Importance of Soil Temperature for the Growth of Temperate Crops under a Tropical Climate and Functional Role of Soil Microbial Diversity.. Microbes and environments, 33(2), 144-150.</t>
+        </is>
+      </c>
+      <c r="D89" s="2" t="inlineStr">
+        <is>
+          <t>A soil cooling system that prepares soil for temperate soil temperatures for the growth of temperate crops under a tropical climate is described herein. Temperate agriculture has been threatened by the negative impact of temperature increases caused by climate change. Soil temperature closely correlates with the growth of temperate crops, and affects plant processes and soil microbial diversity. The present study focuses on the effects of soil temperatures on lettuce growth and soil microbial diversity that maintains the growth of lettuce at low soil temperatures. A model temperate crop, loose leaf lettuce, was grown on eutrophic soil under soil cooling and a number of parameters, such as fresh weight, height, the number of leaves, and root length, were evaluated upon harvest. Under soil cooling, significant differences were observed in the average fresh weight (P&lt;0.05) and positive development of the roots, shoots, and leaves of lettuce. Janthinobacterium (8.142%), Rhodoplanes (1.991%), Arthrospira (1.138%), Flavobacterium (0.857%), Sphingomonas (0.790%), Mycoplana (0.726%), and Pseudomonas (0.688%) were the dominant bacterial genera present in cooled soil. Key soil fungal communities, including Pseudaleuria (18.307%), Phoma (9.968%), Eocronartium (3.527%), Trichosporon (1.791%), and Pyrenochaeta (0.171%), were also recovered from cooled soil. The present results demonstrate that the growth of temperate crops is dependent on soil temperature, which subsequently affects the abundance and diversity of soil microbial communities that maintain the growth of temperate crops at low soil temperatures.</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>480</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Nitratireductor</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="inlineStr">
+        <is>
+          <t>Chai, J., et al. (2020). Purification and characterization of chitin deacetylase active on insoluble chitin from Nitratireductor aquimarinus MCDA3-3.. International journal of biological macromolecules, 152, 922-929.</t>
+        </is>
+      </c>
+      <c r="D90" s="2" t="inlineStr">
+        <is>
+          <t>The chitin deacetylase produced by marine strain Nitratireductor aquimarinus MCDA3-3 (NaCDA) was purified by using ammonium sulfate precipitation, Q Sepharose, and Superdex column chromatography. The purified NaCDA showed 75-fold purity, 50 U/mg specific activity with 28.5% yield. The purified CDA molecular weight was about 36 kDa. The temperature and pH of the purified enzyme were suiting at 30 °C and 8.0, respectively. The NaCDA was highly stable for a wide range of temperature 4 °C-25 °C and pH 6.0-9.0. Besides, increased enzyme activity was observed by introducing metal ions mainly Sr&lt;sup&gt;2+&lt;/sup&gt;, Mg&lt;sup&gt;2+&lt;/sup&gt;, and Na&lt;sup&gt;+&lt;/sup&gt;. The enzyme was founded inhibited by Co&lt;sup&gt;2+&lt;/sup&gt;, Ba&lt;sup&gt;2+&lt;/sup&gt;, and EDTA at the value of 1 mM concentrations. On the other hand, NaCDA was shown an active activity behavior toward glycol chitin and chitin oligomers with a degree of polymerization more than four, any polymer below the chain such as trimer and dimer significantly reduce in the activity rate, and inactive with N-acetylglucosamine. Interestingly, NaCDA showed a high activity rate against insoluble chitins and converting acetyls to deacetylated. The reduction of acetyls from 56.26% and 22.88% of acetyl groups from ɑ-chitin and β-chitin, respectively. Hence, the NaCDA would be applicable in production chitosan toward mass production.</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>494</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Oceaniovalibus</t>
+        </is>
+      </c>
+      <c r="C91" s="2" t="inlineStr"/>
+      <c r="D91" s="2" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>541</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Peptoclostridium</t>
+        </is>
+      </c>
+      <c r="C92" s="2" t="inlineStr">
+        <is>
+          <t>Pereira, F., et al. (2016). Complete genome sequence of &lt;i&gt;Peptoclostridium difficile&lt;/i&gt; strain Z31.. Gut pathogens, 8, 11.</t>
+        </is>
+      </c>
+      <c r="D92" s="2" t="inlineStr">
+        <is>
+          <t>&lt;i&gt;Peptoclostridium&lt;/i&gt; (&lt;i&gt;Clostridium&lt;/i&gt;) &lt;i&gt;difficile&lt;/i&gt; is a spore-forming bacterium responsible for nosocomial infections in humans. It is recognized as an important agent of diarrhea and colitis in several animal species and a possible zoonotic agent. Despite the known importance of &lt;i&gt;P. difficile&lt;/i&gt; infection in humans and animals, no vaccine or other effective measure to control the disease is commercially available. A possible alternative treatment for &lt;i&gt;P. difficile&lt;/i&gt; infection is the use of a nontoxigenic strain of &lt;i&gt;P. difficile&lt;/i&gt; as a competitive exclusion agent. However, a thorough knowledge of this strain is necessary for this purpose. We selected &lt;i&gt;P. difficile&lt;/i&gt; Z31, a nontoxigenic strain (PCR ribotype 009), for investigation because it prevents &lt;i&gt;P. difficile&lt;/i&gt; infection in a hamster model.</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>549</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Phenylobacterium</t>
+        </is>
+      </c>
+      <c r="C93" s="2" t="inlineStr">
+        <is>
+          <t>Pouder, E., et al. (2024). Phenylobacterium ferrooxidans sp. nov., isolated from a sub-surface geothermal aquifer in Iceland.. Systematic and applied microbiology, 48(1), 126578.</t>
+        </is>
+      </c>
+      <c r="D93" s="2" t="inlineStr">
+        <is>
+          <t>A novel bacterial strain, HK31-G&lt;sup&gt;T&lt;/sup&gt;, was isolated from a subsurface geothermal aquifer (Hellisheidi, SW-Iceland) and was characterized using a polyphasic taxonomic approach. Phylogenetic analysis of 16S rRNA gene along with phylogenomic position indicated that the novel strain belongs to the genus Phenylobacterium. Cells are motile Gram-negative thin rods. Physiological characterization showed that strain HK31-G&lt;sup&gt;T&lt;/sup&gt; is a mesophilic bacterium able to grow from 10 to 30 °C, at pH values between 6 and 8 and at NaCl concentrations between 0 and 0.5 %. Optimal growth was observed without sodium chloride at 25 °C and pH 6. Strain HK31-G&lt;sup&gt;T&lt;/sup&gt; is chemoorganoheterotroph and its major saturated fatty acids are C&lt;sub&gt;18:1&lt;/sub&gt;ω7c, C&lt;sub&gt;16&lt;/sub&gt;&lt;sub&gt;:1&lt;/sub&gt;ω6c and C&lt;sub&gt;16:0&lt;/sub&gt;, the predominant quinone is Q-10 and the major polar lipid is phosphatidylglycerol. The new strain also possesses the capacity to use ferrous iron (Fe(II)) as the sole energy source and can also be considered as a chemolithoautotrophic microorganism. The overall genome of strain HK31-G&lt;sup&gt;T&lt;/sup&gt; was estimated to be 4.46 Mbp in size with a DNA G + C content of 67.95 %. Genes involved in iron metabolism were identified, but no genes typically involved in Fe(II)-oxidation were found. According to the overall genome relatedness indices (OGRI) values, six MAGs from groundwater have been assigned to the same species as the new strain HK31-G&lt;sup&gt;T&lt;/sup&gt;. Furthermore, OGRI values between the genome of strain HK31-G&lt;sup&gt;T&lt;/sup&gt; and the genomes of its closest relatives are below the species delineation threshold. Therefore, given the polyphasic approach used, strain HK31-G&lt;sup&gt;T&lt;/sup&gt; represents a novel species of the genus Phenylobacterium, for which the name Phenylobacterium ferrooxidans sp. nov. is proposed. The type strain is HK31-G&lt;sup&gt;T&lt;/sup&gt; (DSM 116432&lt;sup&gt;T&lt;/sup&gt; = UBOCC-M-3429&lt;sup&gt;T&lt;/sup&gt; = LMG 33376&lt;sup&gt;T&lt;/sup&gt;).</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>565</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Porphyromonas</t>
+        </is>
+      </c>
+      <c r="C94" s="2" t="inlineStr">
+        <is>
+          <t>Eduok, U. &amp; Szpunar, J. (2020). &lt;i&gt;In vitro&lt;/i&gt; corrosion studies of stainless-steel dental substrates during &lt;i&gt;Porphyromonas gingivalis&lt;/i&gt; biofilm growth in artificial saliva solutions: providing insights into the role of resident oral bacterium.. RSC advances, 10(52), 31280-31294.</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="inlineStr">
+        <is>
+          <t>Stainless-steel AISI 321 is an effective material for fabricating dental crowns and other implants utilized dental restorative protocols for elderly and pediatric populations. This unique clinical application is possible through the mechanical stability and corrosion-resistance properties of this metallic material. However, stainless-steel dental implants eventually fail, leading to the creation of surface cavities and cracks within their microstructures during persistent mechanical stresses and biocorrosion. In this study, the &lt;i&gt;in vitro&lt;/i&gt; corrosion behaviour of a medical-grade stainless-steel dental substrate was investigated during &lt;i&gt;Porphyromonas gingivalis&lt;/i&gt; biofilm growth process in artificial saliva culture suspension (ASCS). Among the causative bioagents of corrosion, &lt;i&gt;P. gingivalis&lt;/i&gt; was chosen for this study since it is also responsible for oral periodontitis and a major contributing factor to corrosion in most dental implants. Increased &lt;i&gt;P. gingivalis&lt;/i&gt; growth was observed within the incubation period under study as compact cellular clusters fouled the metal surfaces in ASCS media. This led to the corrosion of steel substrates after bacterial growth maturity within 90 days. Corrosion rate increased with higher CFU and bacterial incubation period for all test substrates due to biocorrosion incited by the volatile sulphide products of &lt;i&gt;P. gingivalis&lt;/i&gt; metabolism. The presence of some of these volatile compounds has been observed from experimental evidences. Significant anodic degradation in the forms of localized pitting were also recorded by surface analytical techniques. Residual fluorinated ions within the ASCS media also increased the rate of anodic dissolution due to media acidity. This study has provided extensive insights into the fate of stainless-steel dental crown in oral environments infected by a resident oral bacterium. Influences of oral conditions similar to fluoride-enriched mouthwashes were reflected in a view to understanding the corrosion patterns of stainless-steel dental substrates.</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>584</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Pseudoalteromonas</t>
+        </is>
+      </c>
+      <c r="C95" s="2" t="inlineStr">
+        <is>
+          <t>Liang, Y., Wang, P. &amp; Zhang, D. (2021). Designing a Highly Stable Slippery Organogel on Q235 Carbon Steel for Inhibiting Microbiologically Influenced Corrosion.. ACS applied bio materials, 4(8), 6056-6064.</t>
+        </is>
+      </c>
+      <c r="D95" s="2" t="inlineStr">
+        <is>
+          <t>Microbiologically influenced corrosion (MIC) accelerates the corrosion and degradation of metal materials due to the settlement of microorganisms on the surface. However, environmentally friendly and efficient methods to fabricate antifouling and anticorrosion surfaces are still lacking. Inspired by &lt;i&gt;Nepenthes&lt;/i&gt;, a slippery liquid-infused porous surface (SLIPS) has been proven to be an efficient way to inhibit settlement of microorganisms on the metal surface and the following MIC due to the existence of a mobile defect-free lubricant layer. However, the stability of the lubricant layer and substrate of the SLIPS prevented its long-term antifouling and anticorrosion application. Herein, a highly stable slippery organogel was fabricated by depositing a homogeneous mixture of PDMS (base and curing agent), silicone oil, triethoxyvinylsilane, and SiO&lt;sub&gt;2&lt;/sub&gt; on Q235 and curing in an oven. Triethoxyvinylsilane was not only able to cross-link with the curing agent of PDMS through hydrosilylation but also able to interlink the organogel and Q235 through condensation between the -OH of the metal surface and hydrolyzed siloxane. As a result, the adhesion force between the organogel without triethoxyvinylsilane and the substrate (0.45 MPa) increased to 1.50 MPa for the organogel with triethoxyvinylsilane and SiO&lt;sub&gt;2&lt;/sub&gt;. Also, the tensile strength of the organogel without SiO&lt;sub&gt;2&lt;/sub&gt; (0.97 MPa) increased to 3.88 MPa for the organogel with 2 wt % SiO&lt;sub&gt;2&lt;/sub&gt; because of the high elastic modulus of SiO&lt;sub&gt;2&lt;/sub&gt;, which was important to improving its stability under external force. In addition, the organogel showed stable oil distribution and slippery performance after spinning at 4000 rpm for 30 s. Then, the bacterial settlement demonstrated that the organogel could effectively inhibit &lt;i&gt;Pseudoalteromonas&lt;/i&gt; sp. settlement on the substrate under both static and dynamic conditions. Finally, an electrochemical test indicated that the MIC could be effectively mitigated by the organogel. This study provides an efficient method to fabricate a highly stable slippery surface on a metal surface for its potential application in mitigating MIC.</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>605</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Rhodanobacter</t>
+        </is>
+      </c>
+      <c r="C96" s="2" t="inlineStr">
+        <is>
+          <t>Xia, C., Cheng, W., Ren, M. &amp; Zhu, Y. (2025). Chromium(VI) and nitrate removal from groundwater using biochar-assisted zero valent iron autotrophic bioreduction: Enhancing electron transfer efficiency and reducing EPS accumulation.. Environmental pollution (Barking, Essex : 1987), 364(Pt 1), 125313.</t>
+        </is>
+      </c>
+      <c r="D96" s="2" t="inlineStr">
+        <is>
+          <t>Current strategies primarily utilize heterotrophic or mixotrophic bioreduction for the simultaneous removal of Cr(VI) and NO&lt;sub&gt;3&lt;/sub&gt;&lt;sup&gt;-&lt;/sup&gt; from groundwater. However, given the oligotrophic nature of groundwater, autotrophic bioreduction could be more appropriate, though it remains notably underdeveloped. Here, an autotrophic bioreduction technology utilizing biochar (BC)-assisted zero valent iron (ZVI) is proposed. The pyrolysis temperature of BC was optimized to enhance electron transfer efficiency and reduce extracellular polymeric substances (EPS) accumulation. BC500, with the superior electron transfer capabilities, was the most effective. After an 11-week period, the ZVI + BC500 biotic column still achieved 100% removal efficiency for Cr(VI) and 93.37 ± 0.33% for NO&lt;sub&gt;3&lt;/sub&gt;&lt;sup&gt;-&lt;/sup&gt;, with initial concentrations of 26 mg/L and 50 mg/L, respectively. Its performance significantly surpasses that of ZVI alone, effectively reducing the interference of Cr(VI) on denitrification. The presence of quinone and phenolic compounds in BC500, serving as electron-accepting and electron-donating groups, improves the efficiency of electron transfer between ZVI and microbes. Metagenomic analysis showed an increase in the growth of autotrophic bacteria such as Hydrogenophaga spp. and Rhodanobacter denitrificans, and heterotrophic bacteria including Arenimonas daejeonensis and Chryseobacterium shandongense. The promotion facilitates the expression of genes associated with Cr(VI) reduction (chrR, nemA) and denitrification (narG, nirS). BC500 also enhanced EPS production, which facilitates the adsorption and reduction of Cr(VI), mitigating its inhibitory effects on denitrification. Notably, in the ZVI + BC500 biotic column, the accumulated EPS primarily consists of loosely bound EPS rather than tightly bound EPS, potentially reducing the risk of pore clogging during in-situ groundwater treatment.</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>625</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Roseococcus</t>
+        </is>
+      </c>
+      <c r="C97" s="2" t="inlineStr">
+        <is>
+          <t>Yurkov, V., Jappe, J. &amp; Vermeglio, A. (1996). Tellurite resistance and reduction by obligately aerobic photosynthetic bacteria.. Applied and environmental microbiology, 62(11), 4195-8.</t>
+        </is>
+      </c>
+      <c r="D97" s="2" t="inlineStr">
+        <is>
+          <t>Seven species of obligately aerobic photosynthetic bacteria of the genera Erythromicrobium, Erythrobacter, and Roseococcus demonstrated high-level resistance to tellurite and accumulation of metallic tellurium crystals. High-level resistance without tellurite reduction was observed for Roseococcus thiosulfatophilus and Erythromicrobium ezovicum grown with certain organic carbon sources, implying that tellurite reduction is not essential to confer tellurite resistance.</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>636</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Ruminococcaceae_ucg-005</t>
+        </is>
+      </c>
+      <c r="C98" s="2" t="inlineStr">
+        <is>
+          <t>Liu, X., et al. (2024). Ferulic Acid Relieves the Oxidative Stress Induced by Oxidized Fish Oil in Oriental River Prawn (&lt;i&gt;Macrobrachium nipponense&lt;/i&gt;) with an Emphasis on Lipid Metabolism and Gut Microbiota.. Antioxidants (Basel, Switzerland), 13(12).</t>
+        </is>
+      </c>
+      <c r="D98" s="2" t="inlineStr">
+        <is>
+          <t>To investigate the potential of ferulic acid (FA) in attenuating the deleterious effects of oxidized fish oil (OF) on &lt;i&gt;Macrobrachium nipponense&lt;/i&gt;, four experimental diets were formulated: 3% fresh fish oil (CT group, peroxide value: 2.2 mmol/kg), 3% oxidized fish oil (OF group, peroxide value: 318 mmol/kg), and 3% OF with an additional 160 and 320 mg/kg of FA (OF+FA160 group and OF+FA320 group, respectively). &lt;i&gt;M. nipponense&lt;/i&gt; (initial weight: 0.140 ± 0.015 g) were randomly divided into four groups with six replicates (60 individuals per replicate) and reared for a period of 10 weeks. The results showed that the OF treatments significantly reduced the growth performance, the expression of antioxidant genes in the hepatopancreas, the levels of low-density lipoprotein cholesterol, and the gene expression levels of &lt;i&gt;ACC&lt;/i&gt;, &lt;i&gt;FAS&lt;/i&gt;, &lt;i&gt;FABP10&lt;/i&gt;, &lt;i&gt;ACBP&lt;/i&gt;, &lt;i&gt;G6PDH&lt;/i&gt;, and &lt;i&gt;SCD&lt;/i&gt; in the hepatopancreas (&lt;i&gt;p&lt;/i&gt; &lt; 0.05). OF supplementation significantly increased the levels of high-density lipoprotein cholesterol in hemolymph and the gene expression levels of &lt;i&gt;CPT1&lt;/i&gt; (&lt;i&gt;p&lt;/i&gt; &lt; 0.05). Addition of FA to the OF group significantly increased total bile acids (&lt;i&gt;p&lt;/i&gt; &lt; 0.05). In addition, it was found by Oil Red staining that the proportion of lipid droplets was significantly increased in the OF group (&lt;i&gt;p&lt;/i&gt; &lt; 0.05). However, the lipid droplets were alleviated by FA supplementation in the diet. OF was found to significantly reduce the diversity of intestinal microbiota by 16S rDNA sequencing and significantly increase the Firmicutes/Bacteroidetes (F/B) ratio (&lt;i&gt;p&lt;/i&gt; &lt; 0.05). Functional analysis of gut microbiota also showed that OF reduced lipolysis and led to fat deposition, which is related to gut microbiota. However, this study found that the composition of the gut microbiome of &lt;i&gt;M. nipponense&lt;/i&gt; was changed by the addition of FA in the diet, including an increase in the abundance of &lt;i&gt;Ruminococcaceae UCG-005&lt;/i&gt; and Lachnospiraceae, a reduction in the F/B ratio, and an improvement in lipid metabolism. In conclusion, the OF induced oxidative stress, disturbed the balance of intestinal microbiota, promoted lipid accumulation, and caused disorders of lipid metabolism in &lt;i&gt;M. nipponense&lt;/i&gt; by increasing lipid synthesis and reducing β-oxidation. However, the results of this study highlighted the potential of FA supplementation to modulate intestinal microbial composition, promote bile acid production, and activate genes related to lipid metabolism in the hepatopancreas, ultimately leading to a reduction in lipid deposition in &lt;i&gt;M. nipponense&lt;/i&gt;.</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>657</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Shinella</t>
+        </is>
+      </c>
+      <c r="C99" s="2" t="inlineStr">
+        <is>
+          <t>Chen, X., Yu, T. &amp; Zeng, X. (2024). Functional features of a novel Sb(III)- and As(III)-oxidizing bacterium: Implications for the interactions between bacterial Sb(III) and As(III) oxidation pathways.. Chemosphere, 352, 141385.</t>
+        </is>
+      </c>
+      <c r="D99" s="2" t="inlineStr">
+        <is>
+          <t>Antimony (Sb) and arsenic (As) share similar chemical characteristics and commonly coexist in contaminated environments. It has been reported that the biogeochemical cycles of antimony and arsenic affect each other. However, there is limited understanding regarding microbial coupling between the biogeochemical processes of antimony and arsenic. Here, we aimed to solve this issue. We successfully isolated a novel bacterium, Shinella sp. SbAsOP1, which possesses both Sb(III) and As(III) oxidase, and can effectively oxidize both Sb(III) and As(III) under aerobic and anaerobic conditions. SbAsOP1 exhibits greater aerobic oxidation activity for the oxidation of As(III) or Sb(III) compared to its anaerobic activity. SbAsOP1 also significantly catalyzes the oxidative mobilization of solid-phase Sb(III) under aerobic conditions. The activity of SbAsOP1 in oxidizing solid Sb(III) is 3 times lower than its activity in oxidizing soluble form. It is noteworthy that, in the presence of both Sb(III) and As(III) under aerobic conditions, either As(III) or Sb(III) significantly inhibits the oxidation of Sb(III) or As(III), respectively. In comparison, under anaerobic conditions and in the coexistence of Sb(III) and As(III), As(III) significantly inhibits Sb(III) oxidation, whereas Sb(III) almost completely inhibits As(III) oxidation. These findings suggest that under both aerobic and anaerobic conditions, SbAsOP1 demonstrates a partial preference for Sb(III) oxidation. Additionally, bacterial oxidations of Sb(III) and As(III) mutually inhibit each other to varying degrees. These observations gain a novel understanding of the interplay between the biogeochemical processes of antimony and arsenic.</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>678</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Sphingosinicella</t>
+        </is>
+      </c>
+      <c r="C100" s="2" t="inlineStr"/>
+      <c r="D100" s="2" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>712</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Tepidimonas</t>
+        </is>
+      </c>
+      <c r="C101" s="2" t="inlineStr">
+        <is>
+          <t>Mondal, N., et al. (2024). Aquificae overcomes competition by archaeal thermophiles, and crowding by bacterial mesophiles, to dominate the boiling vent-water of a Trans-Himalayan sulfur-borax spring.. PloS one, 19(10), e0310595.</t>
+        </is>
+      </c>
+      <c r="D101" s="2" t="inlineStr">
+        <is>
+          <t>Trans-Himalayan hot spring waters rich in boron, chlorine, sodium and sulfur (but poor in calcium and silicon) are known based on PCR-amplified 16S rRNA gene sequence data to harbor high diversities of infiltrating bacterial mesophiles. Yet, little is known about the community structure and functions, primary productivity, mutual interactions, and thermal adaptations of the microorganisms present in the steaming waters discharged by these geochemically peculiar spring systems. We revealed these aspects of a bacteria-dominated microbiome (microbial cell density ~8.5 × 104 mL-1; live:dead cell ratio 1.7) thriving in the boiling (85°C) fluid vented by a sulfur-borax spring called Lotus Pond, situated at 4436 m above the mean sea-level, in the Puga valley of eastern Ladakh, on the Changthang plateau. Assembly, annotation, and population-binning of &gt;15-GB metagenomic sequence illuminated the numeral predominance of Aquificae. While members of this phylum accounted for 80% of all 16S rRNA-encoding reads within the metagenomic dataset, 14% of such reads were attributed to Proteobacteria. Post assembly, only 25% of all protein-coding genes identified were attributable to Aquificae, whereas 41% was ascribed to Proteobacteria. Annotation of metagenomic reads encoding 16S rRNAs, and/or PCR-amplified 16S rRNA genes, identified 163 bacterial genera, out of which 66 had been detected in past investigations of Lotus Pond's vent-water via 16S amplicon sequencing. Among these 66, Fervidobacterium, Halomonas, Hydrogenobacter, Paracoccus, Sulfurihydrogenibium, Tepidimonas, Thermus and Thiofaba (or their close phylogenomic relatives) were presently detected as metagenome-assembled genomes (MAGs). Remarkably, the Hydrogenobacter related MAG alone accounted for ~56% of the entire metagenome, even though only 15 out of the 66 genera consistently present in Lotus Pond's vent-water have strains growing in the laboratory at &gt;45°C, reflecting the continued existence of the mesophiles in the ecosystem. Furthermore, the metagenome was replete with genes crucial for thermal adaptation in the context of Lotus Pond's geochemistry and topography. In terms of sequence similarity, a majority of those genes were attributable to phylogenetic relatives of mesophilic bacteria, while functionally they rendered functions such as encoding heat shock proteins, molecular chaperones, and chaperonin complexes; proteins controlling/modulating/inhibiting DNA gyrase; universal stress proteins; methionine sulfoxide reductases; fatty acid desaturases; different toxin-antitoxin systems; enzymes protecting against oxidative damage; proteins conferring flagellar structure/function, chemotaxis, cell adhesion/aggregation, biofilm formation, and quorum sensing. The Lotus Pond Aquificae not only dominated the microbiome numerically but also acted potentially as the main primary producers of the ecosystem, with chemolithotrophic sulfur oxidation (Sox) being the fundamental bioenergetic mechanism, and reductive tricarboxylic acid (rTCA) cycle the predominant carbon fixation pathway. The Lotus Pond metagenome contained several genes directly or indirectly related to virulence functions, biosynthesis of secondary metabolites including antibiotics, antibiotic resistance, and multi-drug efflux pumping. A large proportion of these genes being attributable to Aquificae, and Proteobacteria (very few were ascribed to Archaea), it could be worth exploring in the future whether antibiosis helped the Aquificae overcome niche overlap with other thermophiles (especially those belonging to Archaea), besides exacerbating the bioenergetic costs of thermal endurance for the mesophilic intruders of the ecosystem.</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>725</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Thermus</t>
+        </is>
+      </c>
+      <c r="C102" s="2" t="inlineStr">
+        <is>
+          <t>Suflita, J., Aktas, D., Oldham, A., Perez-Ibarra, B. &amp; Duncan, K. (2012). Molecular tools to track bacteria responsible for fuel deterioration and microbiologically influenced corrosion.. Biofouling, 28(9), 1003-10.</t>
+        </is>
+      </c>
+      <c r="D102" s="2" t="inlineStr">
+        <is>
+          <t>Investigating the susceptibility of various fuels to anaerobic biodegradation has become complicated with the recognition that the fuels themselves are not sterile. Bacterial DNA could be obtained when various fuels were filtered through a hydrophobic teflon (0.22 μm) membrane filter. Bacterial 16S rRNA genes from these preparations were PCR amplified, cloned, and the resulting libraries sequenced to identify the fuel-borne bacterial communities. The most common sequence, found in algal- and camelina-based biofuels as well as in ultra-low sulfur diesel (ULSD) and F76 diesel, was similar to that of a Tumebacillus. The next most common sequence was similar to Methylobacterium and was found in the biofuels and ULSD. Higher level phylogenetic groups included representatives of the Firmicutes (Bacillus, Lactobacillus and Streptococcus), several Actinobacteria, Deinococcus-Thermus, Chloroflexi, Cyanobacteria, Bacteroidetes, Alphaproteobacteria (Methylobacterium and Sphingomonadales), Betaproteobacteria (Oxalobacteraceae and Burkholderiales) and Deltaproteobacteria. All of the fuel-associated bacterial sequences, except those obtained from a few facultative microorganisms, were from aerobes and only remotely affiliated with sequences that resulted from anaerobic successional events evident when ULSD was incubated with a coastal seawater and sediment inoculum. Thus, both traditional and alternate fuel formulations harbor a characteristic microflora, but these microorganisms contributed little to the successional patterns that ultimately resulted in fuel decomposition, sulfide formation and metal biocorrosion. The findings illustrate the value of molecular approaches to track the fate of bacteria that might come in contact with fuels and potentially contribute to corrosion problems throughout the energy value chain.</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>864</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Veillonella</t>
+        </is>
+      </c>
+      <c r="C103" s="2" t="inlineStr">
+        <is>
+          <t>Noar, J., et al. (2003). An in vitro study into the corrosion of intra-oral magnets in the presence of dental amalgam.. European journal of orthodontics, 25(6), 615-9.</t>
+        </is>
+      </c>
+      <c r="D103" s="2" t="inlineStr">
+        <is>
+          <t>The aim of this investigation was to study the corrosion behaviour and products of uncoated neodymium-iron-boron magnets in the presence of dental amalgam. Microcosm plaques were grown on discs of neodymium-iron-boron magnets or amalgam in a constant depth film fermentor. The biofilms were supplied with artificial saliva and growth was determined by viable counting. The results showed that the neodymium-iron-boron magnets corroded with an average daily weight loss of 0.115 +/- 0.032 per cent. However, when the magnets were in close proximity to the amalgam the amount of corrosion was reduced to a daily loss of 0.066 +/- 0.023 per cent. The highest loss of constituent elements from the corrosion products of the magnets was observed for iron. The composition of the microcosm plaques altered markedly between the two materials with less streptococci and more Veillonella spp. present in the biofilms grown on magnets in the presence of amalgam. The corrosion of neodymium-iron-boron magnets is limited and in the presence of amalgam is reduced further. This suggests that amalgam present in the mouth will not cause an increased clinical risk in terms of biocompatibility with neodymium-iron-boron magnets.</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>871</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Xanthobacter</t>
+        </is>
+      </c>
+      <c r="C104" s="2" t="inlineStr">
+        <is>
+          <t>He, J., et al. (2024). Distinguishing contributions of diverse sediment components to vanadium transport, immobilization and transformation in aquifer.. Water research, 265, 122248.</t>
+        </is>
+      </c>
+      <c r="D104" s="2" t="inlineStr">
+        <is>
+          <t>Vanadium (V) occurs in environment naturally and anthropogenically, but little has been understood about its environmental behavior in groundwater aquifer with sediments. This study investigated the pentavalent V [V(V)] transport and transformation under the influence of different sediment components (minerals, organic matter, and microorganisms) through column experiments. All these components played pivotal roles in V immobilization. The synergistic effects of sediment components enhanced V retention compared to individual component. Mineral components, particularly those containing carbonates and metal oxides, predominantly influenced V(V) transport as indicated by XRD analysis. Organic matter, especially under low pH conditions, induced particle aggregation, thereby inhibiting the transport of V(V). The V K-edge X-ray absorption near-edge structure spectroscopy revealed the formation of tetravalent V[V(IV)] in treatments involving organic matter and microorganisms. Notably, organic matter exhibited the capability to directly reduce V(V). The introduction of microorganisms restricted V(V) transfer. V(V) reducing genera (e.g., Brevundimonas, Arenimonas, Xanthobacter) were detected, achieving V(V) reduction to insoluble V(IV). V(V) bioreduction was improved by minerals that promote microbial metabolism with enhanced electron transfer, or by organic matter that increases levels of intracellular nicotinamide adenine dinucleotide and extracellular polymeric substances. This study specifies the contributions of different sediment components to the transportation and transformation of V, deepening our understanding of V biogeochemistry in groundwater aquifer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>872</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Xanthomonadaceae_bacterium_wwh73</t>
+        </is>
+      </c>
+      <c r="C105" s="2" t="inlineStr">
+        <is>
+          <t>Chung, K., Fujiki, I. &amp; Okabe, S. (2011). Effect of formation of biofilms and chemical scale on the cathode electrode on the performance of a continuous two-chamber microbial fuel cell.. Bioresource technology, 102(1), 355-60.</t>
+        </is>
+      </c>
+      <c r="D105" s="2" t="inlineStr">
+        <is>
+          <t>A two-chamber MFC system was operated continuously for more than 500 days to evaluate effects of biofilm and chemical scale formation on the cathode electrode on power generation. A stable power density of 0.57 W/m(2) was attained after 200 days operation. However, the power density decreased drastically to 0.2 W/m(2) after the cathodic biofilm and chemical scale were removed. As the cathodic biofilm and chemical scale partially accumulated on the cathode, the power density gradually recovered with time. Microbial community structure of the cathodic biofilm was analyzed based on 16S rRNA clone libraries. The clones closely related to Xanthomonadaceae bacterium and Xanthomonas sp. in the Gammaproteobacteria subdivision were most frequently retrieved from the cathodic biofilm. Results of the SEM-EDX analysis revealed that the cation species (Na(+) and Ca(2+)) were main constituents of chemical scale, indicating that these cations diffused from the anode chamber through the Nafion membrane. However, an excess accumulation of the biofilm and chemical scale on the cathode exhibited adverse effects on the power generation due to a decrease in the active cathode surface area and an increase in diffusion resistance for oxygen. Thus, it is important to properly control the formation of chemical scale and biofilm on the cathode during long-term operation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Azospira</t>
+        </is>
+      </c>
+      <c r="C106" s="2" t="inlineStr">
+        <is>
+          <t>Gregoire, P., et al. (2014). Control of sulfidogenesis through bio-oxidation of H2S coupled to (per)chlorate reduction.. Environmental microbiology reports, 6(6), 558-64.</t>
+        </is>
+      </c>
+      <c r="D106" s="2" t="inlineStr">
+        <is>
+          <t>We investigated H2S attenuation by dissimilatory perchlorate-reducing bacteria (DPRB). All DPRB tested oxidized H2S coupled to (per)chlorate reduction without sustaining growth. H2S was preferentially utilized over organic electron donors resulting in an enriched (34S)-elemental sulfur product. Electron microscopy revealed elemental sulfur production in the cytoplasm and on the cell surface of the DPRB Azospira suillum. Based on our results, we propose a novel hybrid enzymatic-abiotic mechanism for H2S oxidation similar to that recently proposed for nitrate-dependent Fe(II) oxidation. The results of this study have implications for the control of biosouring and biocorrosion in a range of industrial environments.</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Brachybacterium</t>
+        </is>
+      </c>
+      <c r="C107" s="2" t="inlineStr">
+        <is>
+          <t>Liu, Y., et al. (2018). Evaluation of compost, vegetable and food waste as amendments to improve the composting of NaOH/NaClO-contaminated poultry manure.. PloS one, 13(10), e0205112.</t>
+        </is>
+      </c>
+      <c r="D107" s="2" t="inlineStr">
+        <is>
+          <t>Regular usage of NaOH/NaClO disinfectants results in high sodium salt and alkalinity of poultry manure. This study compared three amendments: vegetable waste (V), food waste (F) and mature compost (C) for their ability to improve the composting of NaOH/NaClO-contaminated poultry manure. C compost resulted in the highest compost temperatures (p&lt;0.001) and greatest reduction in OM, TC, TN and NH4-N (p&lt;0.05). C and V composts were more efficient at lowering extractable-Na (ext-Na) and electrical conductivity (EC) than F (p&lt;0.05). Maturity was primarily indicated by NH4-N, EC and ext-Na. Bacterial dynamics was profoundly influenced by NH4-N, EC and TC, with the decrease leading to discriminate genera shift from Sinibacillus and Thiopseudomonas to Brevbacterium, Brachybacterium, and Microbacterium. These findings suggest that mature compost was more desirable amendment than vegetable and food waste in the composting of NaOH/NaClO-contaminated poultry manure, and the decrease of ext-Na indicated compost maturity but did not influence bacterial dynamics.</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Bulleidia</t>
+        </is>
+      </c>
+      <c r="C108" s="2" t="inlineStr">
+        <is>
+          <t>Jia, Y., et al. (2021). Association Between Oral Microbiota and Cigarette Smoking in the Chinese Population.. Frontiers in cellular and infection microbiology, 11, 658203.</t>
+        </is>
+      </c>
+      <c r="D108" s="2" t="inlineStr">
+        <is>
+          <t>The oral microbiota has been observed to be influenced by cigarette smoking and linked to several human diseases. However, research on the effect of cigarette smoking on the oral microbiota has not been systematically conducted in the Chinese population. We profiled the oral microbiota of 316 healthy subjects in the Chinese population by 16S rRNA gene sequencing. The alpha diversity of oral microbiota was different between never smokers and smokers (&lt;i&gt;P&lt;/i&gt; = 0.002). Several bacterial taxa were first reported to be associated with cigarette smoking by LEfSe analysis, including &lt;i&gt;Moryella&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 1.56E-04), &lt;i&gt;Bulleidia&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 1.65E-06), and &lt;i&gt;Moraxella&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 3.52E-02) at the genus level and &lt;i&gt;Rothia dentocariosa&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 1.55E-02), &lt;i&gt;Prevotella melaninogenica&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 8.48E-08), &lt;i&gt;Prevotella pallens&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 4.13E-03), &lt;i&gt;Bulleidia moorei&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 1.79E-06), &lt;i&gt;Rothia aeria&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 3.83E-06), &lt;i&gt;Actinobacillus parahaemolyticus&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 2.28E-04), and &lt;i&gt;Haemophilus parainfluenzae&lt;/i&gt; (&lt;i&gt;q&lt;/i&gt; = 4.82E-02) at the species level. Two nitrite-producing bacteria that can increase the acidity of the oral cavity, &lt;i&gt;Actinomyces&lt;/i&gt; and &lt;i&gt;Veillonella&lt;/i&gt;, were also enriched in smokers with FDR-adjusted &lt;i&gt;q&lt;/i&gt;-values of 3.62E-06 and 1.10E-06, respectively. Notably, we observed that two acid production-related pathways, amino acid-related enzymes (&lt;i&gt;q&lt;/i&gt; = 6.19E-05) and amino sugar and nucleotide sugar metabolism (&lt;i&gt;q&lt;/i&gt; = 2.63E-06), were increased in smokers by PICRUSt analysis. Finally, the co-occurrence analysis demonstrated that smoker-enriched bacteria were significantly positively associated with each other and were negatively correlated with the bacteria decreased in smokers. Our results suggested that cigarette smoking may affect oral health by creating a different environment by altering bacterial abundance, connections among oral microbiota, and the microbiota and their metabolic function.</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Cellulosimicrobium</t>
+        </is>
+      </c>
+      <c r="C109" s="2" t="inlineStr">
+        <is>
+          <t>Wyszkowska, J., Borowik, A., Zaborowska, M. &amp; Kucharski, J. (2022). Sensitivity of &lt;i&gt;Zea mays&lt;/i&gt; and Soil Microorganisms to the Toxic Effect of Chromium (VI).. International journal of molecular sciences, 24(1).</t>
+        </is>
+      </c>
+      <c r="D109" s="2" t="inlineStr">
+        <is>
+          <t>Chromium is used in many settings, and hence, it can easily enter the natural environment. It exists in several oxidation states. In soil, depending on its oxidation-reduction potential, it can occur in bivalent, trivalent or hexavalent forms. Hexavalent chromium compounds are cancerogenic to humans. The aim of this study was to determine the effect of Cr(VI) on the structure of bacteria and fungi in soil, to find out how this effect is modified by humic acids and to determine the response of &lt;i&gt;Zea mays&lt;/i&gt; to this form of chromium. A pot experiment was conducted to answer the above questions. &lt;i&gt;Zea mays&lt;/i&gt; was sown in natural soil and soil polluted with Cr(VI) in an amount of 60 mg kg&lt;sup&gt;-1&lt;/sup&gt; d.m. Both soils were treated with humic acids in the form of HumiAgra preparation. The ecophysiological and genetic diversity of bacteria and fungi was assayed in soil under maize (not sown with &lt;i&gt;Zea mays&lt;/i&gt;). In addition, the following were determined: yield of maize, greenness index, index of tolerance to chromium, translocation index and accumulation of chromium in the plant. It has been determined that Cr(VI) significantly distorts the growth and development of &lt;i&gt;Zea mays&lt;/i&gt;, while humic acids completely neutralize its toxic effect on the plant. This element had an adverse effect on the development of bacteria of the genera &lt;i&gt;Cellulosimicrobium&lt;/i&gt;, &lt;i&gt;Kaistobacter&lt;/i&gt;, &lt;i&gt;Rhodanobacter&lt;/i&gt;, &lt;i&gt;Rhodoplanes&lt;/i&gt; and &lt;i&gt;Nocardioides&lt;/i&gt; and fungi of the genera &lt;i&gt;Chaetomium and Humicola&lt;/i&gt;. Soil contamination with Cr(VI) significantly diminished the genetic diversity and richness of bacteria and the ecophysiological diversity of fungi. The negative impact of Cr(VI) on the diversity of bacteria and fungi was mollified by &lt;i&gt;Zea mays&lt;/i&gt; and the application of humic acids.</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Clostridium</t>
+        </is>
+      </c>
+      <c r="C110" s="2" t="inlineStr">
+        <is>
+          <t>Ramos Monroy, O., Ruiz Ordaz, N., Hernández Gayosso, M., Juárez Ramírez, C. &amp; Galíndez Mayer, J. (2019). The corrosion process caused by the activity of the anaerobic sporulated bacterium Clostridium celerecrescens on API XL 52 steel.. Environmental science and pollution research international, 26(29), 29991-30002.</t>
+        </is>
+      </c>
+      <c r="D110" s="2" t="inlineStr">
+        <is>
+          <t>The microbial corrosion of oil and gas pipes is one of the problems occurring in the oil industry. Various mechanisms explaining microbial corrosion have been demonstrated. Commonly, biocorrosion is attributed to sulfate-reducing bacteria. Also, it has recently been reported that microbial species can connect their electron transport system to metal electrodes. In this research, two spore-forming bacteria isolated in different years from a gas pipeline were identified by biochemical techniques and by 16S rDNA amplification, sequencing, and comparison with the NCBI database. Isolates were also compared between them using molecular techniques as the restriction patterns, unique for 16S rDNA (ARDRA), and the profile of the amplified bit from the genomic DNA, using an unspecific primer (RAPD). The results obtained showed that both isolates corresponded to Clostridium celerecrescens with a 99% similarity according to the sequence reported on the NCBI database. Also, the ARDRA and RAPD electrophoretic profiles of both strains were identical, and no plasmids were found in the strains. Thus, it can be settled that this bacterium is persistent in the environment prevailing in gas pipelines. Also, it was demonstrated that the bacterial secretion of organic acids contributes to the pitting and general biocorrosion of API XL 52 steel. The rates of corrosion obtained, approximately after 40 days, were correlated with the presence and metabolic activity of C. celerecrescens on the metallic surfaces.</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Corynebacterium</t>
+        </is>
+      </c>
+      <c r="C111" s="2" t="inlineStr">
+        <is>
+          <t>Zhang, D., et al. (2024). The relationships of metals exposure and disturbance of the vaginal microbiota with the risk of PROM: Results from a birth cohort study.. Ecotoxicology and environmental safety, 289, 117420.</t>
+        </is>
+      </c>
+      <c r="D111" s="2" t="inlineStr">
+        <is>
+          <t>The vaginal microbiota is proposed to be associated with reproductive health. Exposure to metals during pregnancy is a risk factor for premature rupture of membranes (PROM). PROM can lead to serious maternal complications, thus, identifying the cause and therapeutic targets for it is crucial. However, the role of vaginal microbiota in the association between metals exposure and the risk of PROM are not clear. Based on a prospective birth cohort study including 668 pregnant women, maternal blood levels of 15 metals in the first trimester (n=668) and microbiota of vaginal secretions in the third trimester (n=244) were assessed. The metals that significantly associated with the risk of PROM were screened out via four statistical models, the top three were barium (Ba), chromium (Cr) and thallium (Tl) according to their weight indices. The results from the BKMR model showed a positive association of the mixture (Ba, Cr and Tl) with the risk of PROM. PROM and non-PROM were characterised by different beta diversities, moreover, the relative abundances of Bifidobacterium, Corynebacterium and Collinsella were statistically and negatively related to the risk of PROM [the adjusted odds ratios (ORs) and 95 % confidence intervals (CIs) were 0.06 (0.00, 0.82), 0.32 (0.14, 0.74) and 0.50 (0.30, 0.84), respectively]. On the other hand, women with different levels of Ba exposure were also characterised by different beta diversities (p value = 0.047); and blood Ba levels were also negatively associated with the relative abundances of Collinsella; additionally, Cr levels were positively associated with alpha diversity indices [Shannon index: β (95 % CI) = 0.25 (0.01, 0.50); Simpson index: β (95 % CI) = 0.08 (0.00, 0.17), respectively]. The results from mediation analysis showed the proportion of the relationship between Ba exposure and PROM risk mediated by the relative abundance of Collinsella was 26.4 %. Further verification analysis exploring the potential cause of the above phenomenon indicated that the neutrophil count, one of blood inflammation indicators for PROM, was higher in women with the absence of Collinsella (p value = 0.039), moreover, the cumulative hazard of PROM for women with the presence of Collinsella was also significantly lower than that of those without Collinsella (p value = 0.007). Collectively, the changes in the diversity and composition of the bacterial community, especially the reduction in Collinsella abundance caused by metal exposure, may be related to the occurrence of PROM, which provides a new microbiota-based perspective for intervention in metal exposure-related PROM. Confirming these relationships and determining the possible processes at play will require more investigation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>354</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Halomonas</t>
+        </is>
+      </c>
+      <c r="C112" s="2" t="inlineStr">
+        <is>
+          <t>Li, C., et al. (2024). Effect of Halomonas titanicae on fluctuating water-line corrosion of EH40 steel.. Bioelectrochemistry (Amsterdam, Netherlands), 158, 108703.</t>
+        </is>
+      </c>
+      <c r="D112" s="2" t="inlineStr">
+        <is>
+          <t>The fluctuating water-line corrosion of EH40 steel in sterile and biotic media was investigated with a wire beam electrode. When the coupons were partially immersed in the sterile medium, the position of the low water-line acted as the cathodic zone and the area below the low water-line constantly served as the main anodic zone. The thin electrolyte layers with uneven thickness promoted the galvanic current of the region below the low water-line. Different from the sterile environment, the metabolism of Halomonas titanica with oxygen as the final electron acceptor reduced the dissolved oxygen concentration, which resulted in the position of the low water-line acting as the anodic zone.</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>408</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Legionella</t>
+        </is>
+      </c>
+      <c r="C113" s="2" t="inlineStr">
+        <is>
+          <t>Spencer-Williams, I., Meyer, M., DePas, W., Elliott, E. &amp; Haig, S. (2023). Assessing the Impacts of Lead Corrosion Control on the Microbial Ecology and Abundance of Drinking-Water-Associated Pathogens in a Full-Scale Drinking Water Distribution System.. Environmental science &amp; technology, 57(48), 20360-20369.</t>
+        </is>
+      </c>
+      <c r="D113" s="2" t="inlineStr">
+        <is>
+          <t>Increases in phosphate availability in drinking water distribution systems (DWDSs) from the use of phosphate-based corrosion control strategies may result in nutrient and microbial community composition shifts in the DWDS. This study assessed the year-long impacts of full-scale DWDS orthophosphate addition on both the microbial ecology and density of drinking-water-associated pathogens that infect the immunocompromised (DWPIs). Using 16S rRNA gene amplicon sequencing and droplet digital PCR, drinking water microbial community composition and DWPI density were examined. Microbial community composition analysis suggested significant compositional changes after the orthophosphate addition. Significant increases in total bacterial density were observed after orthophosphate addition, likely driven by a 2 log 10 increase in nontuberculous mycobacteria (NTM). Linear effect models confirmed the importance of phosphate addition with phosphorus concentration explaining 17% and 12% of the variance in NTM and &lt;i&gt;L. pneumophila&lt;/i&gt; density, respectively. To elucidate the impact of phosphate on NTM aggregation, a comparison of planktonic and aggregate fractions of NTM cultures grown at varying phosphate concentrations was conducted. Aggregation assay results suggested that higher phosphate concentrations cause more disaggregation, and the interaction between phosphate and NTM is species specific. This work reveals new insight into the consequences of orthophosphate application on the DWDS microbiome and highlights the importance of proactively monitoring the DWDS for DWPIs.</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>471</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Mycoplana</t>
+        </is>
+      </c>
+      <c r="C114" s="2" t="inlineStr">
+        <is>
+          <t>Sabri, N., Zakaria, Z., Mohamad, S., Jaafar, A. &amp; Hara, H. (2018). Importance of Soil Temperature for the Growth of Temperate Crops under a Tropical Climate and Functional Role of Soil Microbial Diversity.. Microbes and environments, 33(2), 144-150.</t>
+        </is>
+      </c>
+      <c r="D114" s="2" t="inlineStr">
+        <is>
+          <t>A soil cooling system that prepares soil for temperate soil temperatures for the growth of temperate crops under a tropical climate is described herein. Temperate agriculture has been threatened by the negative impact of temperature increases caused by climate change. Soil temperature closely correlates with the growth of temperate crops, and affects plant processes and soil microbial diversity. The present study focuses on the effects of soil temperatures on lettuce growth and soil microbial diversity that maintains the growth of lettuce at low soil temperatures. A model temperate crop, loose leaf lettuce, was grown on eutrophic soil under soil cooling and a number of parameters, such as fresh weight, height, the number of leaves, and root length, were evaluated upon harvest. Under soil cooling, significant differences were observed in the average fresh weight (P&lt;0.05) and positive development of the roots, shoots, and leaves of lettuce. Janthinobacterium (8.142%), Rhodoplanes (1.991%), Arthrospira (1.138%), Flavobacterium (0.857%), Sphingomonas (0.790%), Mycoplana (0.726%), and Pseudomonas (0.688%) were the dominant bacterial genera present in cooled soil. Key soil fungal communities, including Pseudaleuria (18.307%), Phoma (9.968%), Eocronartium (3.527%), Trichosporon (1.791%), and Pyrenochaeta (0.171%), were also recovered from cooled soil. The present results demonstrate that the growth of temperate crops is dependent on soil temperature, which subsequently affects the abundance and diversity of soil microbial communities that maintain the growth of temperate crops at low soil temperatures.</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>497</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Oerskovia</t>
+        </is>
+      </c>
+      <c r="C115" s="2" t="inlineStr">
+        <is>
+          <t>Rana, S., Kumar, A., Walia, S., Berven, K., Cumper, K. &amp; Walia, S. (2011). Isolation of Tn1546-like elements in vancomycin-resistant Enterococcus faecium isolated from wood frogs: an emerging risk for zoonotic bacterial infections to humans.. Journal of applied microbiology, 110(1), 35-43.</t>
+        </is>
+      </c>
+      <c r="D115" s="2" t="inlineStr">
+        <is>
+          <t>Isolation and characterization of vancomycin-resistant enterococci (VRE), mainly Enterococcus faecium, from the faecal pellet of wood frogs (Rana sylvatica).</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>512</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Oxobacter</t>
+        </is>
+      </c>
+      <c r="C116" s="2" t="inlineStr"/>
+      <c r="D116" s="2" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>526</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Paracoccus</t>
+        </is>
+      </c>
+      <c r="C117" s="2" t="inlineStr">
+        <is>
+          <t>Huber, B., Drewes, J., Lin, K., König, R. &amp; Müller, E. (2014). Revealing biogenic sulfuric acid corrosion in sludge digesters: detection of sulfur-oxidizing bacteria within full-scale digesters.. Water science and technology : a journal of the International Association on Water Pollution Research, 70(8), 1405-11.</t>
+        </is>
+      </c>
+      <c r="D117" s="2" t="inlineStr">
+        <is>
+          <t>Biogenic sulfuric acid corrosion (BSA) is a costly problem affecting both sewerage infrastructure and sludge handling facilities such as digesters. The aim of this study was to verify BSA in full-scale digesters by identifying the microorganisms involved in the concrete corrosion process, that is, sulfate-reducing (SRB) and sulfur-oxidizing bacteria (SOB). To investigate the SRB and SOB communities, digester sludge and biofilm samples were collected. SRB diversity within digester sludge was studied by applying polymerase chain reaction-denaturing gradient gel electrophoresis (PCR-DGGE) targeting the dsrB-gene (dissimilatory sulfite reductase beta subunit). To reveal SOB diversity, cultivation dependent and independent techniques were applied. The SRB diversity studies revealed different uncultured SRB, confirming SRB activity and H2S production. Comparable DGGE profiles were obtained from the different sludges, demonstrating the presence of similar SRB species. By cultivation, three pure SOB strains from the digester headspace were obtained including Acidithiobacillus thiooxidans, Thiomonas intermedia and Thiomonas perometabolis. These organisms were also detected with PCR-DGGE in addition to two new SOB: Thiobacillus thioparus and Paracoccus solventivorans. The SRB and SOB responsible for BSA were identified within five different digesters, demonstrating that BSA is a problem occurring not only in sewer systems but also in sludge digesters. In addition, the presence of different SOB species was successfully associated with the progression of microbial corrosion.</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>581</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Psb-m-3</t>
+        </is>
+      </c>
+      <c r="C118" s="2" t="inlineStr">
+        <is>
+          <t>Pei, Y., Yu, Z., Ji, J., Khan, A. &amp; Li, X. (2018). Microbial Community Structure and Function Indicate the Severity of Chromium Contamination of the Yellow River.. Frontiers in microbiology, 9, 38.</t>
+        </is>
+      </c>
+      <c r="D118" s="2" t="inlineStr">
+        <is>
+          <t>The Yellow River is the most important water resource in northern China. In the recent past, heavy metal contamination has become severe due to industrial processes and other anthropogenic activities. In this study, riparian soil samples with varying levels of chromium (Cr) pollution severity were collected along the Gansu industrial reach of the Yellow River, including samples from uncontaminated sites (XC, XGU), slightly contaminated sites (LJX, XGD), and heavily contaminated sites (CG, XG). The Cr concentrations of these samples varied from 83.83 mg⋅kg&lt;sup&gt;-1&lt;/sup&gt; (XGU) to 506.58 mg⋅kg&lt;sup&gt;-1&lt;/sup&gt; (XG). The chromate [Cr (VI)] reducing ability in the soils collected in this study followed the sequence of the heavily contaminated &gt; slightly contaminated &gt; the un-contaminated. Common Cr remediation genes &lt;i&gt;chrA&lt;/i&gt; and &lt;i&gt;yieF&lt;/i&gt; were detected in the XG and CG samples. qRT-PCR results showed that the expression of &lt;i&gt;chrA&lt;/i&gt; was up-regulated four and threefold in XG and CG samples, respectively, whereas the expression of &lt;i&gt;yieF&lt;/i&gt; was up-regulated 66- and 7-fold in the same samples after 30 min treatment with Cr (VI). The copy numbers of &lt;i&gt;chrA&lt;/i&gt; and &lt;i&gt;yieF&lt;/i&gt; didn't change after 35 days incubation with Cr (VI). The microbial communities in the Cr contaminated sampling sites were different from those in the uncontaminated samples. Especially, the relative abundances of &lt;i&gt;Firmicutes&lt;/i&gt; and &lt;i&gt;Bacteroidetes&lt;/i&gt; were higher while &lt;i&gt;Actinobacteria&lt;/i&gt; was lower in the contaminated group than uncontaminated group. Further, potential indicator species, related to Cr such as Cr-remediation genera (&lt;i&gt;Geobacter, PSB-M-3, Flavobacterium&lt;/i&gt;, and &lt;i&gt;Methanosarcina&lt;/i&gt;); the Cr-sensitive genera (&lt;i&gt;Skermanella, Iamia, Arthrobacter&lt;/i&gt;, and &lt;i&gt;Candidatus Nitrososphaera&lt;/i&gt;) were also identified. These data revealed that Cr shifted microbial composition and function. Further, Cr (VI) reducing ability could be related with the expression of Cr remediation genes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t>584</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Pseudoalteromonas</t>
+        </is>
+      </c>
+      <c r="C119" s="2" t="inlineStr">
+        <is>
+          <t>Liang, Y., Wang, P. &amp; Zhang, D. (2021). Designing a Highly Stable Slippery Organogel on Q235 Carbon Steel for Inhibiting Microbiologically Influenced Corrosion.. ACS applied bio materials, 4(8), 6056-6064.</t>
+        </is>
+      </c>
+      <c r="D119" s="2" t="inlineStr">
+        <is>
+          <t>Microbiologically influenced corrosion (MIC) accelerates the corrosion and degradation of metal materials due to the settlement of microorganisms on the surface. However, environmentally friendly and efficient methods to fabricate antifouling and anticorrosion surfaces are still lacking. Inspired by &lt;i&gt;Nepenthes&lt;/i&gt;, a slippery liquid-infused porous surface (SLIPS) has been proven to be an efficient way to inhibit settlement of microorganisms on the metal surface and the following MIC due to the existence of a mobile defect-free lubricant layer. However, the stability of the lubricant layer and substrate of the SLIPS prevented its long-term antifouling and anticorrosion application. Herein, a highly stable slippery organogel was fabricated by depositing a homogeneous mixture of PDMS (base and curing agent), silicone oil, triethoxyvinylsilane, and SiO&lt;sub&gt;2&lt;/sub&gt; on Q235 and curing in an oven. Triethoxyvinylsilane was not only able to cross-link with the curing agent of PDMS through hydrosilylation but also able to interlink the organogel and Q235 through condensation between the -OH of the metal surface and hydrolyzed siloxane. As a result, the adhesion force between the organogel without triethoxyvinylsilane and the substrate (0.45 MPa) increased to 1.50 MPa for the organogel with triethoxyvinylsilane and SiO&lt;sub&gt;2&lt;/sub&gt;. Also, the tensile strength of the organogel without SiO&lt;sub&gt;2&lt;/sub&gt; (0.97 MPa) increased to 3.88 MPa for the organogel with 2 wt % SiO&lt;sub&gt;2&lt;/sub&gt; because of the high elastic modulus of SiO&lt;sub&gt;2&lt;/sub&gt;, which was important to improving its stability under external force. In addition, the organogel showed stable oil distribution and slippery performance after spinning at 4000 rpm for 30 s. Then, the bacterial settlement demonstrated that the organogel could effectively inhibit &lt;i&gt;Pseudoalteromonas&lt;/i&gt; sp. settlement on the substrate under both static and dynamic conditions. Finally, an electrochemical test indicated that the MIC could be effectively mitigated by the organogel. This study provides an efficient method to fabricate a highly stable slippery surface on a metal surface for its potential application in mitigating MIC.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>